<commit_message>
PPU is added to the bus
An example for the ppu is added
</commit_message>
<xml_diff>
--- a/Instruction Set/InstSet.xlsx
+++ b/Instruction Set/InstSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cemal\Documents\GitHub\myCPU\Instruction Set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA8C9FB-CC40-4B12-BC1C-C1C9CEDAF76F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CAB141-0396-4723-9D56-C2D4FE927F46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Decoder" sheetId="3" r:id="rId1"/>
@@ -5750,7 +5750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D60C82-07C4-4D43-9229-4AF7BD948FF4}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -6278,7 +6278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New test cases are added
</commit_message>
<xml_diff>
--- a/Instruction Set/InstSet.xlsx
+++ b/Instruction Set/InstSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cemal\Documents\GitHub\myCPU\Instruction Set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CAB141-0396-4723-9D56-C2D4FE927F46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1B3F69-375A-4892-85C5-E967AC78A135}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Decoder" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="300">
   <si>
     <t>S3</t>
   </si>
@@ -833,6 +833,102 @@
   </si>
   <si>
     <t>#LRL|#LRH</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>0010</t>
+  </si>
+  <si>
+    <t>0011</t>
+  </si>
+  <si>
+    <t>0100</t>
+  </si>
+  <si>
+    <t>0101</t>
+  </si>
+  <si>
+    <t>0110</t>
+  </si>
+  <si>
+    <t>0111</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>1010</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>1101</t>
+  </si>
+  <si>
+    <t>1110</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>EQ</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>LO</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>VS</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>GT</t>
+  </si>
+  <si>
+    <t>LE</t>
+  </si>
+  <si>
+    <t>VC</t>
   </si>
 </sst>
 </file>
@@ -2087,9 +2183,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2108,19 +2201,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2165,6 +2246,207 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="57" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="29" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="58" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="27" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="30" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="44" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="46" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="40" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="33" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="38" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="37" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2174,67 +2456,13 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="57" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="29" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="58" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="27" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="40" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="33" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="46" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2245,138 +2473,6 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="30" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="44" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="38" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="37" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2678,7 +2774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0587EB1-1C15-4BDC-B095-DE818FDD326C}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
@@ -3616,7 +3712,7 @@
   <dimension ref="A1:U45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T3" sqref="T3:T6"/>
+      <selection activeCell="S1" sqref="S1:U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4676,25 +4772,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F660B940-324A-409A-9742-8BFC9B3A5F3A}">
-  <dimension ref="A1:T34"/>
+  <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W20" sqref="W20:Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="11.42578125" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" customWidth="1"/>
+    <col min="1" max="4" width="11.42578125" style="87" customWidth="1"/>
+    <col min="5" max="19" width="9.140625" style="87"/>
+    <col min="20" max="20" width="9.140625" style="87" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="87"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="125" t="s">
+    <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="187" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="127"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="189"/>
       <c r="E1" s="91">
         <v>15</v>
       </c>
@@ -4744,7 +4842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="95" t="s">
         <v>237</v>
       </c>
@@ -4760,928 +4858,1207 @@
       <c r="E2" s="98">
         <v>0</v>
       </c>
-      <c r="F2" s="99">
+      <c r="F2" s="121">
         <v>0</v>
       </c>
-      <c r="G2" s="99">
+      <c r="G2" s="121">
         <v>0</v>
       </c>
-      <c r="H2" s="100">
+      <c r="H2" s="99">
         <v>0</v>
       </c>
-      <c r="I2" s="101">
+      <c r="I2" s="100">
         <v>0</v>
       </c>
-      <c r="J2" s="192" t="s">
+      <c r="J2" s="125" t="s">
         <v>123</v>
       </c>
-      <c r="K2" s="193"/>
-      <c r="L2" s="194"/>
-      <c r="M2" s="167" t="s">
+      <c r="K2" s="126"/>
+      <c r="L2" s="127"/>
+      <c r="M2" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="168"/>
-      <c r="O2" s="168"/>
-      <c r="P2" s="168"/>
-      <c r="Q2" s="168" t="s">
+      <c r="N2" s="182"/>
+      <c r="O2" s="182"/>
+      <c r="P2" s="182"/>
+      <c r="Q2" s="182" t="s">
         <v>124</v>
       </c>
-      <c r="R2" s="168"/>
-      <c r="S2" s="168"/>
-      <c r="T2" s="169"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="102" t="s">
+      <c r="R2" s="182"/>
+      <c r="S2" s="182"/>
+      <c r="T2" s="183"/>
+      <c r="W2" s="87" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y2" s="87" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="101" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="103" t="s">
+      <c r="B3" s="102" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="103" t="s">
+      <c r="C3" s="102" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="104" t="s">
+      <c r="D3" s="103" t="s">
         <v>128</v>
       </c>
-      <c r="E3" s="105">
+      <c r="E3" s="104">
         <v>0</v>
       </c>
-      <c r="F3" s="106">
+      <c r="F3" s="122">
         <v>0</v>
       </c>
-      <c r="G3" s="106">
+      <c r="G3" s="122">
         <v>0</v>
       </c>
-      <c r="H3" s="107">
+      <c r="H3" s="124">
         <v>0</v>
       </c>
-      <c r="I3" s="108">
+      <c r="I3" s="105">
         <v>1</v>
       </c>
-      <c r="J3" s="170" t="s">
+      <c r="J3" s="128" t="s">
         <v>123</v>
       </c>
-      <c r="K3" s="170"/>
-      <c r="L3" s="195"/>
-      <c r="M3" s="161" t="s">
+      <c r="K3" s="128"/>
+      <c r="L3" s="129"/>
+      <c r="M3" s="184" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="170"/>
-      <c r="O3" s="170"/>
-      <c r="P3" s="170"/>
-      <c r="Q3" s="170" t="s">
+      <c r="N3" s="128"/>
+      <c r="O3" s="128"/>
+      <c r="P3" s="128"/>
+      <c r="Q3" s="128" t="s">
         <v>124</v>
       </c>
-      <c r="R3" s="170"/>
-      <c r="S3" s="170"/>
-      <c r="T3" s="171"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="112" t="s">
+      <c r="R3" s="128"/>
+      <c r="S3" s="128"/>
+      <c r="T3" s="185"/>
+      <c r="W3" s="87" t="s">
+        <v>268</v>
+      </c>
+      <c r="X3" s="87" t="s">
+        <v>284</v>
+      </c>
+      <c r="Y3" s="87" t="s">
+        <v>268</v>
+      </c>
+      <c r="Z3" s="87" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="107" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="146" t="s">
+      <c r="B4" s="130" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="147"/>
-      <c r="D4" s="148"/>
-      <c r="E4" s="105">
+      <c r="C4" s="152"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="104">
         <v>0</v>
       </c>
-      <c r="F4" s="106">
+      <c r="F4" s="122">
         <v>0</v>
       </c>
-      <c r="G4" s="106">
+      <c r="G4" s="122">
         <v>0</v>
       </c>
-      <c r="H4" s="107">
+      <c r="H4" s="124">
         <v>1</v>
       </c>
-      <c r="I4" s="108">
+      <c r="I4" s="105">
         <v>0</v>
       </c>
-      <c r="J4" s="110">
+      <c r="J4" s="120">
         <v>0</v>
       </c>
-      <c r="K4" s="170" t="s">
+      <c r="K4" s="128" t="s">
         <v>123</v>
       </c>
-      <c r="L4" s="195"/>
-      <c r="M4" s="161" t="s">
+      <c r="L4" s="129"/>
+      <c r="M4" s="184" t="s">
         <v>122</v>
       </c>
-      <c r="N4" s="170"/>
-      <c r="O4" s="170"/>
-      <c r="P4" s="170"/>
-      <c r="Q4" s="170" t="s">
+      <c r="N4" s="128"/>
+      <c r="O4" s="128"/>
+      <c r="P4" s="128"/>
+      <c r="Q4" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="R4" s="170"/>
-      <c r="S4" s="170"/>
-      <c r="T4" s="171"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="149" t="s">
+      <c r="R4" s="128"/>
+      <c r="S4" s="128"/>
+      <c r="T4" s="185"/>
+      <c r="W4" s="87" t="s">
+        <v>269</v>
+      </c>
+      <c r="X4" s="87" t="s">
+        <v>285</v>
+      </c>
+      <c r="Y4" s="87" t="s">
+        <v>269</v>
+      </c>
+      <c r="Z4" s="87" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="193" t="s">
         <v>243</v>
       </c>
-      <c r="B5" s="150"/>
-      <c r="C5" s="150"/>
-      <c r="D5" s="151"/>
-      <c r="E5" s="105">
+      <c r="B5" s="194"/>
+      <c r="C5" s="194"/>
+      <c r="D5" s="195"/>
+      <c r="E5" s="104">
         <v>0</v>
       </c>
-      <c r="F5" s="106">
+      <c r="F5" s="122">
         <v>0</v>
       </c>
-      <c r="G5" s="106">
+      <c r="G5" s="122">
         <v>0</v>
       </c>
-      <c r="H5" s="107">
+      <c r="H5" s="124">
         <v>1</v>
       </c>
-      <c r="I5" s="109">
+      <c r="I5" s="123">
         <v>0</v>
       </c>
-      <c r="J5" s="107">
+      <c r="J5" s="124">
         <v>1</v>
       </c>
-      <c r="K5" s="162" t="s">
+      <c r="K5" s="165" t="s">
         <v>171</v>
       </c>
-      <c r="L5" s="161"/>
-      <c r="M5" s="158" t="s">
+      <c r="L5" s="184"/>
+      <c r="M5" s="186" t="s">
         <v>124</v>
       </c>
-      <c r="N5" s="159"/>
-      <c r="O5" s="159"/>
-      <c r="P5" s="161"/>
-      <c r="Q5" s="158" t="s">
+      <c r="N5" s="166"/>
+      <c r="O5" s="166"/>
+      <c r="P5" s="184"/>
+      <c r="Q5" s="186" t="s">
         <v>172</v>
       </c>
-      <c r="R5" s="159"/>
-      <c r="S5" s="159"/>
-      <c r="T5" s="160"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="172" t="s">
+      <c r="R5" s="166"/>
+      <c r="S5" s="166"/>
+      <c r="T5" s="167"/>
+      <c r="W5" s="87" t="s">
+        <v>270</v>
+      </c>
+      <c r="X5" s="87" t="s">
+        <v>286</v>
+      </c>
+      <c r="Y5" s="87" t="s">
+        <v>270</v>
+      </c>
+      <c r="Z5" s="87" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="150" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="173"/>
-      <c r="C6" s="146" t="s">
+      <c r="B6" s="151"/>
+      <c r="C6" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="148"/>
-      <c r="E6" s="105">
+      <c r="D6" s="131"/>
+      <c r="E6" s="104">
         <v>0</v>
       </c>
-      <c r="F6" s="106">
+      <c r="F6" s="122">
         <v>0</v>
       </c>
-      <c r="G6" s="106">
+      <c r="G6" s="122">
         <v>0</v>
       </c>
-      <c r="H6" s="107">
+      <c r="H6" s="124">
         <v>1</v>
       </c>
-      <c r="I6" s="108">
+      <c r="I6" s="105">
         <v>1</v>
       </c>
-      <c r="J6" s="107" t="s">
+      <c r="J6" s="124" t="s">
         <v>123</v>
       </c>
-      <c r="K6" s="162" t="s">
+      <c r="K6" s="165" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="159"/>
-      <c r="M6" s="159"/>
-      <c r="N6" s="161"/>
-      <c r="O6" s="158" t="s">
+      <c r="L6" s="166"/>
+      <c r="M6" s="166"/>
+      <c r="N6" s="184"/>
+      <c r="O6" s="186" t="s">
         <v>130</v>
       </c>
-      <c r="P6" s="159"/>
-      <c r="Q6" s="159"/>
-      <c r="R6" s="159"/>
-      <c r="S6" s="159"/>
-      <c r="T6" s="160"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="137" t="s">
+      <c r="P6" s="166"/>
+      <c r="Q6" s="166"/>
+      <c r="R6" s="166"/>
+      <c r="S6" s="166"/>
+      <c r="T6" s="167"/>
+      <c r="W6" s="87" t="s">
+        <v>271</v>
+      </c>
+      <c r="X6" s="87" t="s">
+        <v>287</v>
+      </c>
+      <c r="Y6" s="87" t="s">
+        <v>271</v>
+      </c>
+      <c r="Z6" s="87" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="136" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="138"/>
-      <c r="C7" s="138"/>
-      <c r="D7" s="139"/>
+      <c r="B7" s="137"/>
+      <c r="C7" s="137"/>
+      <c r="D7" s="138"/>
       <c r="E7" s="134">
         <v>0</v>
       </c>
-      <c r="F7" s="131">
+      <c r="F7" s="132">
         <v>0</v>
       </c>
-      <c r="G7" s="131">
+      <c r="G7" s="132">
         <v>1</v>
       </c>
-      <c r="H7" s="128">
+      <c r="H7" s="148">
         <v>0</v>
       </c>
-      <c r="I7" s="163" t="s">
+      <c r="I7" s="142" t="s">
         <v>122</v>
       </c>
-      <c r="J7" s="153"/>
-      <c r="K7" s="153"/>
-      <c r="L7" s="164"/>
-      <c r="M7" s="152" t="s">
+      <c r="J7" s="143"/>
+      <c r="K7" s="143"/>
+      <c r="L7" s="144"/>
+      <c r="M7" s="153" t="s">
         <v>129</v>
       </c>
-      <c r="N7" s="153"/>
-      <c r="O7" s="153"/>
-      <c r="P7" s="153"/>
-      <c r="Q7" s="153"/>
-      <c r="R7" s="153"/>
-      <c r="S7" s="153"/>
+      <c r="N7" s="143"/>
+      <c r="O7" s="143"/>
+      <c r="P7" s="143"/>
+      <c r="Q7" s="143"/>
+      <c r="R7" s="143"/>
+      <c r="S7" s="143"/>
       <c r="T7" s="154"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="140"/>
-      <c r="B8" s="141"/>
-      <c r="C8" s="141"/>
-      <c r="D8" s="142"/>
-      <c r="E8" s="136"/>
+      <c r="W7" s="87" t="s">
+        <v>272</v>
+      </c>
+      <c r="X7" s="87" t="s">
+        <v>288</v>
+      </c>
+      <c r="Y7" s="87" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z7" s="87" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="139"/>
+      <c r="B8" s="140"/>
+      <c r="C8" s="140"/>
+      <c r="D8" s="141"/>
+      <c r="E8" s="135"/>
       <c r="F8" s="133"/>
       <c r="G8" s="133"/>
-      <c r="H8" s="130"/>
-      <c r="I8" s="165"/>
-      <c r="J8" s="156"/>
-      <c r="K8" s="156"/>
-      <c r="L8" s="166"/>
+      <c r="H8" s="149"/>
+      <c r="I8" s="145"/>
+      <c r="J8" s="146"/>
+      <c r="K8" s="146"/>
+      <c r="L8" s="147"/>
       <c r="M8" s="155"/>
-      <c r="N8" s="156"/>
-      <c r="O8" s="156"/>
-      <c r="P8" s="156"/>
-      <c r="Q8" s="156"/>
-      <c r="R8" s="156"/>
-      <c r="S8" s="156"/>
-      <c r="T8" s="157"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="172" t="s">
+      <c r="N8" s="146"/>
+      <c r="O8" s="146"/>
+      <c r="P8" s="146"/>
+      <c r="Q8" s="146"/>
+      <c r="R8" s="146"/>
+      <c r="S8" s="146"/>
+      <c r="T8" s="156"/>
+      <c r="W8" s="87" t="s">
+        <v>273</v>
+      </c>
+      <c r="X8" s="87" t="s">
+        <v>289</v>
+      </c>
+      <c r="Y8" s="87" t="s">
+        <v>273</v>
+      </c>
+      <c r="Z8" s="87" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="150" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="173"/>
-      <c r="C9" s="146" t="s">
+      <c r="B9" s="151"/>
+      <c r="C9" s="130" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="148"/>
-      <c r="E9" s="105">
+      <c r="D9" s="131"/>
+      <c r="E9" s="104">
         <v>0</v>
       </c>
-      <c r="F9" s="106">
+      <c r="F9" s="122">
         <v>0</v>
       </c>
-      <c r="G9" s="106">
+      <c r="G9" s="122">
         <v>1</v>
       </c>
-      <c r="H9" s="107">
+      <c r="H9" s="124">
         <v>1</v>
       </c>
-      <c r="I9" s="108">
+      <c r="I9" s="105">
         <v>0</v>
       </c>
-      <c r="J9" s="107" t="s">
+      <c r="J9" s="124" t="s">
         <v>123</v>
       </c>
-      <c r="K9" s="162" t="s">
+      <c r="K9" s="165" t="s">
         <v>131</v>
       </c>
-      <c r="L9" s="159"/>
-      <c r="M9" s="159"/>
-      <c r="N9" s="159"/>
-      <c r="O9" s="159"/>
-      <c r="P9" s="159"/>
-      <c r="Q9" s="159"/>
-      <c r="R9" s="159"/>
-      <c r="S9" s="159"/>
-      <c r="T9" s="160"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="172" t="s">
+      <c r="L9" s="166"/>
+      <c r="M9" s="166"/>
+      <c r="N9" s="166"/>
+      <c r="O9" s="166"/>
+      <c r="P9" s="166"/>
+      <c r="Q9" s="166"/>
+      <c r="R9" s="166"/>
+      <c r="S9" s="166"/>
+      <c r="T9" s="167"/>
+      <c r="W9" s="87" t="s">
+        <v>274</v>
+      </c>
+      <c r="X9" s="87" t="s">
+        <v>290</v>
+      </c>
+      <c r="Y9" s="87" t="s">
+        <v>274</v>
+      </c>
+      <c r="Z9" s="87" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="150" t="s">
         <v>231</v>
       </c>
-      <c r="B10" s="147"/>
-      <c r="C10" s="147"/>
-      <c r="D10" s="148"/>
-      <c r="E10" s="105">
+      <c r="B10" s="152"/>
+      <c r="C10" s="152"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="104">
         <v>0</v>
       </c>
-      <c r="F10" s="106">
+      <c r="F10" s="122">
         <v>0</v>
       </c>
-      <c r="G10" s="106">
+      <c r="G10" s="122">
         <v>1</v>
       </c>
-      <c r="H10" s="107">
+      <c r="H10" s="124">
         <v>1</v>
       </c>
-      <c r="I10" s="111">
+      <c r="I10" s="106">
         <v>1</v>
       </c>
-      <c r="J10" s="182" t="s">
+      <c r="J10" s="168" t="s">
         <v>137</v>
       </c>
-      <c r="K10" s="182"/>
-      <c r="L10" s="182"/>
-      <c r="M10" s="182"/>
-      <c r="N10" s="182"/>
-      <c r="O10" s="182"/>
-      <c r="P10" s="182"/>
-      <c r="Q10" s="182"/>
-      <c r="R10" s="182"/>
-      <c r="S10" s="182"/>
-      <c r="T10" s="183"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="137" t="s">
+      <c r="K10" s="168"/>
+      <c r="L10" s="168"/>
+      <c r="M10" s="168"/>
+      <c r="N10" s="168"/>
+      <c r="O10" s="168"/>
+      <c r="P10" s="168"/>
+      <c r="Q10" s="168"/>
+      <c r="R10" s="168"/>
+      <c r="S10" s="168"/>
+      <c r="T10" s="169"/>
+      <c r="W10" s="87" t="s">
+        <v>275</v>
+      </c>
+      <c r="X10" s="87" t="s">
+        <v>291</v>
+      </c>
+      <c r="Y10" s="87" t="s">
+        <v>275</v>
+      </c>
+      <c r="Z10" s="87" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="136" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="138"/>
-      <c r="C11" s="138"/>
-      <c r="D11" s="139"/>
+      <c r="B11" s="137"/>
+      <c r="C11" s="137"/>
+      <c r="D11" s="138"/>
       <c r="E11" s="134">
         <v>0</v>
       </c>
-      <c r="F11" s="131">
+      <c r="F11" s="132">
         <v>1</v>
       </c>
-      <c r="G11" s="131">
+      <c r="G11" s="132">
         <v>0</v>
       </c>
-      <c r="H11" s="128">
+      <c r="H11" s="148">
         <v>0</v>
       </c>
-      <c r="I11" s="163" t="s">
+      <c r="I11" s="142" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="153"/>
-      <c r="K11" s="153"/>
-      <c r="L11" s="164"/>
-      <c r="M11" s="152" t="s">
+      <c r="J11" s="143"/>
+      <c r="K11" s="143"/>
+      <c r="L11" s="144"/>
+      <c r="M11" s="153" t="s">
         <v>129</v>
       </c>
-      <c r="N11" s="153"/>
-      <c r="O11" s="153"/>
-      <c r="P11" s="153"/>
-      <c r="Q11" s="153"/>
-      <c r="R11" s="153"/>
-      <c r="S11" s="153"/>
+      <c r="N11" s="143"/>
+      <c r="O11" s="143"/>
+      <c r="P11" s="143"/>
+      <c r="Q11" s="143"/>
+      <c r="R11" s="143"/>
+      <c r="S11" s="143"/>
       <c r="T11" s="154"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="140"/>
-      <c r="B12" s="141"/>
-      <c r="C12" s="141"/>
-      <c r="D12" s="142"/>
-      <c r="E12" s="136"/>
+      <c r="W11" s="87" t="s">
+        <v>276</v>
+      </c>
+      <c r="X11" s="87" t="s">
+        <v>292</v>
+      </c>
+      <c r="Y11" s="87" t="s">
+        <v>276</v>
+      </c>
+      <c r="Z11" s="87" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="139"/>
+      <c r="B12" s="140"/>
+      <c r="C12" s="140"/>
+      <c r="D12" s="141"/>
+      <c r="E12" s="135"/>
       <c r="F12" s="133"/>
       <c r="G12" s="133"/>
-      <c r="H12" s="130"/>
-      <c r="I12" s="165"/>
-      <c r="J12" s="156"/>
-      <c r="K12" s="156"/>
-      <c r="L12" s="166"/>
+      <c r="H12" s="149"/>
+      <c r="I12" s="145"/>
+      <c r="J12" s="146"/>
+      <c r="K12" s="146"/>
+      <c r="L12" s="147"/>
       <c r="M12" s="155"/>
-      <c r="N12" s="156"/>
-      <c r="O12" s="156"/>
-      <c r="P12" s="156"/>
-      <c r="Q12" s="156"/>
-      <c r="R12" s="156"/>
-      <c r="S12" s="156"/>
-      <c r="T12" s="157"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="137" t="s">
+      <c r="N12" s="146"/>
+      <c r="O12" s="146"/>
+      <c r="P12" s="146"/>
+      <c r="Q12" s="146"/>
+      <c r="R12" s="146"/>
+      <c r="S12" s="146"/>
+      <c r="T12" s="156"/>
+      <c r="W12" s="87" t="s">
+        <v>277</v>
+      </c>
+      <c r="X12" s="87" t="s">
+        <v>299</v>
+      </c>
+      <c r="Y12" s="87" t="s">
+        <v>277</v>
+      </c>
+      <c r="Z12" s="87" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="136" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="138"/>
-      <c r="C13" s="138"/>
-      <c r="D13" s="139"/>
+      <c r="B13" s="137"/>
+      <c r="C13" s="137"/>
+      <c r="D13" s="138"/>
       <c r="E13" s="134">
         <v>0</v>
       </c>
-      <c r="F13" s="131">
+      <c r="F13" s="132">
         <v>1</v>
       </c>
-      <c r="G13" s="131">
+      <c r="G13" s="132">
         <v>0</v>
       </c>
-      <c r="H13" s="128">
+      <c r="H13" s="148">
         <v>1</v>
       </c>
-      <c r="I13" s="163" t="s">
+      <c r="I13" s="142" t="s">
         <v>44</v>
       </c>
-      <c r="J13" s="153"/>
-      <c r="K13" s="153"/>
-      <c r="L13" s="164"/>
-      <c r="M13" s="152" t="s">
+      <c r="J13" s="143"/>
+      <c r="K13" s="143"/>
+      <c r="L13" s="144"/>
+      <c r="M13" s="153" t="s">
         <v>129</v>
       </c>
-      <c r="N13" s="153"/>
-      <c r="O13" s="153"/>
-      <c r="P13" s="153"/>
-      <c r="Q13" s="153"/>
-      <c r="R13" s="153"/>
-      <c r="S13" s="153"/>
+      <c r="N13" s="143"/>
+      <c r="O13" s="143"/>
+      <c r="P13" s="143"/>
+      <c r="Q13" s="143"/>
+      <c r="R13" s="143"/>
+      <c r="S13" s="143"/>
       <c r="T13" s="154"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="140"/>
-      <c r="B14" s="141"/>
-      <c r="C14" s="141"/>
-      <c r="D14" s="142"/>
-      <c r="E14" s="136"/>
+      <c r="W13" s="87" t="s">
+        <v>278</v>
+      </c>
+      <c r="X13" s="87" t="s">
+        <v>293</v>
+      </c>
+      <c r="Y13" s="87" t="s">
+        <v>278</v>
+      </c>
+      <c r="Z13" s="87" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="139"/>
+      <c r="B14" s="140"/>
+      <c r="C14" s="140"/>
+      <c r="D14" s="141"/>
+      <c r="E14" s="135"/>
       <c r="F14" s="133"/>
       <c r="G14" s="133"/>
-      <c r="H14" s="130"/>
-      <c r="I14" s="165"/>
-      <c r="J14" s="156"/>
-      <c r="K14" s="156"/>
-      <c r="L14" s="166"/>
+      <c r="H14" s="149"/>
+      <c r="I14" s="145"/>
+      <c r="J14" s="146"/>
+      <c r="K14" s="146"/>
+      <c r="L14" s="147"/>
       <c r="M14" s="155"/>
-      <c r="N14" s="156"/>
-      <c r="O14" s="156"/>
-      <c r="P14" s="156"/>
-      <c r="Q14" s="156"/>
-      <c r="R14" s="156"/>
-      <c r="S14" s="156"/>
-      <c r="T14" s="157"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="137" t="s">
+      <c r="N14" s="146"/>
+      <c r="O14" s="146"/>
+      <c r="P14" s="146"/>
+      <c r="Q14" s="146"/>
+      <c r="R14" s="146"/>
+      <c r="S14" s="146"/>
+      <c r="T14" s="156"/>
+      <c r="W14" s="87" t="s">
+        <v>279</v>
+      </c>
+      <c r="X14" s="87" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y14" s="87" t="s">
+        <v>279</v>
+      </c>
+      <c r="Z14" s="87" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="136" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="138"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="139"/>
+      <c r="B15" s="137"/>
+      <c r="C15" s="137"/>
+      <c r="D15" s="138"/>
       <c r="E15" s="134">
         <v>0</v>
       </c>
-      <c r="F15" s="131">
+      <c r="F15" s="132">
         <v>1</v>
       </c>
-      <c r="G15" s="128">
+      <c r="G15" s="148">
         <v>1</v>
       </c>
-      <c r="H15" s="163" t="s">
+      <c r="H15" s="142" t="s">
         <v>123</v>
       </c>
-      <c r="I15" s="153"/>
-      <c r="J15" s="153"/>
-      <c r="K15" s="164"/>
-      <c r="L15" s="152" t="s">
+      <c r="I15" s="143"/>
+      <c r="J15" s="143"/>
+      <c r="K15" s="144"/>
+      <c r="L15" s="153" t="s">
         <v>132</v>
       </c>
-      <c r="M15" s="153"/>
-      <c r="N15" s="164"/>
-      <c r="O15" s="152" t="s">
+      <c r="M15" s="143"/>
+      <c r="N15" s="144"/>
+      <c r="O15" s="153" t="s">
         <v>133</v>
       </c>
-      <c r="P15" s="153"/>
-      <c r="Q15" s="164"/>
-      <c r="R15" s="152" t="s">
+      <c r="P15" s="143"/>
+      <c r="Q15" s="144"/>
+      <c r="R15" s="153" t="s">
         <v>134</v>
       </c>
-      <c r="S15" s="153"/>
+      <c r="S15" s="143"/>
       <c r="T15" s="154"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="143"/>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="145"/>
-      <c r="E16" s="135"/>
-      <c r="F16" s="132"/>
-      <c r="G16" s="129"/>
-      <c r="H16" s="184"/>
-      <c r="I16" s="175"/>
-      <c r="J16" s="175"/>
-      <c r="K16" s="176"/>
-      <c r="L16" s="174"/>
-      <c r="M16" s="175"/>
-      <c r="N16" s="176"/>
-      <c r="O16" s="174"/>
-      <c r="P16" s="175"/>
-      <c r="Q16" s="176"/>
-      <c r="R16" s="174"/>
-      <c r="S16" s="175"/>
-      <c r="T16" s="180"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="143"/>
-      <c r="B17" s="144"/>
-      <c r="C17" s="144"/>
-      <c r="D17" s="145"/>
-      <c r="E17" s="135"/>
-      <c r="F17" s="132"/>
-      <c r="G17" s="129"/>
-      <c r="H17" s="184"/>
-      <c r="I17" s="175"/>
-      <c r="J17" s="175"/>
-      <c r="K17" s="176"/>
-      <c r="L17" s="174"/>
-      <c r="M17" s="175"/>
-      <c r="N17" s="176"/>
-      <c r="O17" s="174"/>
-      <c r="P17" s="175"/>
-      <c r="Q17" s="176"/>
-      <c r="R17" s="174"/>
-      <c r="S17" s="175"/>
-      <c r="T17" s="180"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="140"/>
-      <c r="B18" s="141"/>
-      <c r="C18" s="141"/>
-      <c r="D18" s="142"/>
-      <c r="E18" s="136"/>
+      <c r="W15" s="87" t="s">
+        <v>280</v>
+      </c>
+      <c r="X15" s="87" t="s">
+        <v>295</v>
+      </c>
+      <c r="Y15" s="87" t="s">
+        <v>280</v>
+      </c>
+      <c r="Z15" s="87" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="171"/>
+      <c r="B16" s="172"/>
+      <c r="C16" s="172"/>
+      <c r="D16" s="173"/>
+      <c r="E16" s="192"/>
+      <c r="F16" s="191"/>
+      <c r="G16" s="190"/>
+      <c r="H16" s="170"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="157"/>
+      <c r="M16" s="158"/>
+      <c r="N16" s="159"/>
+      <c r="O16" s="157"/>
+      <c r="P16" s="158"/>
+      <c r="Q16" s="159"/>
+      <c r="R16" s="157"/>
+      <c r="S16" s="158"/>
+      <c r="T16" s="163"/>
+      <c r="W16" s="87" t="s">
+        <v>281</v>
+      </c>
+      <c r="X16" s="87" t="s">
+        <v>296</v>
+      </c>
+      <c r="Y16" s="87" t="s">
+        <v>281</v>
+      </c>
+      <c r="Z16" s="87" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="171"/>
+      <c r="B17" s="172"/>
+      <c r="C17" s="172"/>
+      <c r="D17" s="173"/>
+      <c r="E17" s="192"/>
+      <c r="F17" s="191"/>
+      <c r="G17" s="190"/>
+      <c r="H17" s="170"/>
+      <c r="I17" s="158"/>
+      <c r="J17" s="158"/>
+      <c r="K17" s="159"/>
+      <c r="L17" s="157"/>
+      <c r="M17" s="158"/>
+      <c r="N17" s="159"/>
+      <c r="O17" s="157"/>
+      <c r="P17" s="158"/>
+      <c r="Q17" s="159"/>
+      <c r="R17" s="157"/>
+      <c r="S17" s="158"/>
+      <c r="T17" s="163"/>
+      <c r="W17" s="87" t="s">
+        <v>282</v>
+      </c>
+      <c r="X17" s="87" t="s">
+        <v>297</v>
+      </c>
+      <c r="Y17" s="87" t="s">
+        <v>282</v>
+      </c>
+      <c r="Z17" s="87" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="139"/>
+      <c r="B18" s="140"/>
+      <c r="C18" s="140"/>
+      <c r="D18" s="141"/>
+      <c r="E18" s="135"/>
       <c r="F18" s="133"/>
-      <c r="G18" s="130"/>
-      <c r="H18" s="165"/>
-      <c r="I18" s="156"/>
-      <c r="J18" s="156"/>
-      <c r="K18" s="166"/>
+      <c r="G18" s="149"/>
+      <c r="H18" s="145"/>
+      <c r="I18" s="146"/>
+      <c r="J18" s="146"/>
+      <c r="K18" s="147"/>
       <c r="L18" s="155"/>
-      <c r="M18" s="156"/>
-      <c r="N18" s="166"/>
+      <c r="M18" s="146"/>
+      <c r="N18" s="147"/>
       <c r="O18" s="155"/>
-      <c r="P18" s="156"/>
-      <c r="Q18" s="166"/>
+      <c r="P18" s="146"/>
+      <c r="Q18" s="147"/>
       <c r="R18" s="155"/>
-      <c r="S18" s="156"/>
-      <c r="T18" s="157"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="137" t="s">
+      <c r="S18" s="146"/>
+      <c r="T18" s="156"/>
+      <c r="W18" s="87" t="s">
+        <v>283</v>
+      </c>
+      <c r="X18" s="87" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y18" s="87" t="s">
+        <v>283</v>
+      </c>
+      <c r="Z18" s="87" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="136" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="138"/>
-      <c r="C19" s="138"/>
-      <c r="D19" s="139"/>
-      <c r="E19" s="188">
+      <c r="B19" s="137"/>
+      <c r="C19" s="137"/>
+      <c r="D19" s="138"/>
+      <c r="E19" s="177">
         <v>1</v>
       </c>
-      <c r="F19" s="163" t="s">
+      <c r="F19" s="142" t="s">
         <v>123</v>
       </c>
-      <c r="G19" s="153"/>
-      <c r="H19" s="153"/>
-      <c r="I19" s="164"/>
-      <c r="J19" s="152" t="s">
+      <c r="G19" s="143"/>
+      <c r="H19" s="143"/>
+      <c r="I19" s="144"/>
+      <c r="J19" s="153" t="s">
         <v>132</v>
       </c>
-      <c r="K19" s="153"/>
-      <c r="L19" s="164"/>
-      <c r="M19" s="152" t="s">
+      <c r="K19" s="143"/>
+      <c r="L19" s="144"/>
+      <c r="M19" s="153" t="s">
         <v>129</v>
       </c>
-      <c r="N19" s="153"/>
-      <c r="O19" s="153"/>
-      <c r="P19" s="153"/>
-      <c r="Q19" s="153"/>
-      <c r="R19" s="153"/>
-      <c r="S19" s="153"/>
+      <c r="N19" s="143"/>
+      <c r="O19" s="143"/>
+      <c r="P19" s="143"/>
+      <c r="Q19" s="143"/>
+      <c r="R19" s="143"/>
+      <c r="S19" s="143"/>
       <c r="T19" s="154"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="143"/>
-      <c r="B20" s="144"/>
-      <c r="C20" s="144"/>
-      <c r="D20" s="145"/>
-      <c r="E20" s="189"/>
-      <c r="F20" s="184"/>
-      <c r="G20" s="175"/>
-      <c r="H20" s="175"/>
-      <c r="I20" s="176"/>
-      <c r="J20" s="174"/>
-      <c r="K20" s="175"/>
-      <c r="L20" s="176"/>
-      <c r="M20" s="174"/>
-      <c r="N20" s="175"/>
-      <c r="O20" s="175"/>
-      <c r="P20" s="175"/>
-      <c r="Q20" s="175"/>
-      <c r="R20" s="175"/>
-      <c r="S20" s="175"/>
-      <c r="T20" s="180"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="143"/>
-      <c r="B21" s="144"/>
-      <c r="C21" s="144"/>
-      <c r="D21" s="145"/>
-      <c r="E21" s="189"/>
-      <c r="F21" s="184"/>
-      <c r="G21" s="175"/>
-      <c r="H21" s="175"/>
-      <c r="I21" s="176"/>
-      <c r="J21" s="174"/>
-      <c r="K21" s="175"/>
-      <c r="L21" s="176"/>
-      <c r="M21" s="174"/>
-      <c r="N21" s="175"/>
-      <c r="O21" s="175"/>
-      <c r="P21" s="175"/>
-      <c r="Q21" s="175"/>
-      <c r="R21" s="175"/>
-      <c r="S21" s="175"/>
-      <c r="T21" s="180"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="143"/>
-      <c r="B22" s="144"/>
-      <c r="C22" s="144"/>
-      <c r="D22" s="145"/>
-      <c r="E22" s="189"/>
-      <c r="F22" s="184"/>
-      <c r="G22" s="175"/>
-      <c r="H22" s="175"/>
-      <c r="I22" s="176"/>
-      <c r="J22" s="174"/>
-      <c r="K22" s="175"/>
-      <c r="L22" s="176"/>
-      <c r="M22" s="174"/>
-      <c r="N22" s="175"/>
-      <c r="O22" s="175"/>
-      <c r="P22" s="175"/>
-      <c r="Q22" s="175"/>
-      <c r="R22" s="175"/>
-      <c r="S22" s="175"/>
-      <c r="T22" s="180"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="143"/>
-      <c r="B23" s="144"/>
-      <c r="C23" s="144"/>
-      <c r="D23" s="145"/>
-      <c r="E23" s="189"/>
-      <c r="F23" s="184"/>
-      <c r="G23" s="175"/>
-      <c r="H23" s="175"/>
-      <c r="I23" s="176"/>
-      <c r="J23" s="174"/>
-      <c r="K23" s="175"/>
-      <c r="L23" s="176"/>
-      <c r="M23" s="174"/>
-      <c r="N23" s="175"/>
-      <c r="O23" s="175"/>
-      <c r="P23" s="175"/>
-      <c r="Q23" s="175"/>
-      <c r="R23" s="175"/>
-      <c r="S23" s="175"/>
-      <c r="T23" s="180"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="143"/>
-      <c r="B24" s="144"/>
-      <c r="C24" s="144"/>
-      <c r="D24" s="145"/>
-      <c r="E24" s="189"/>
-      <c r="F24" s="184"/>
-      <c r="G24" s="175"/>
-      <c r="H24" s="175"/>
-      <c r="I24" s="176"/>
-      <c r="J24" s="174"/>
-      <c r="K24" s="175"/>
-      <c r="L24" s="176"/>
-      <c r="M24" s="174"/>
-      <c r="N24" s="175"/>
-      <c r="O24" s="175"/>
-      <c r="P24" s="175"/>
-      <c r="Q24" s="175"/>
-      <c r="R24" s="175"/>
-      <c r="S24" s="175"/>
-      <c r="T24" s="180"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="143"/>
-      <c r="B25" s="144"/>
-      <c r="C25" s="144"/>
-      <c r="D25" s="145"/>
-      <c r="E25" s="189"/>
-      <c r="F25" s="184"/>
-      <c r="G25" s="175"/>
-      <c r="H25" s="175"/>
-      <c r="I25" s="176"/>
-      <c r="J25" s="174"/>
-      <c r="K25" s="175"/>
-      <c r="L25" s="176"/>
-      <c r="M25" s="174"/>
-      <c r="N25" s="175"/>
-      <c r="O25" s="175"/>
-      <c r="P25" s="175"/>
-      <c r="Q25" s="175"/>
-      <c r="R25" s="175"/>
-      <c r="S25" s="175"/>
-      <c r="T25" s="180"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="143"/>
-      <c r="B26" s="144"/>
-      <c r="C26" s="144"/>
-      <c r="D26" s="145"/>
-      <c r="E26" s="189"/>
-      <c r="F26" s="184"/>
-      <c r="G26" s="175"/>
-      <c r="H26" s="175"/>
-      <c r="I26" s="176"/>
-      <c r="J26" s="174"/>
-      <c r="K26" s="175"/>
-      <c r="L26" s="176"/>
-      <c r="M26" s="174"/>
-      <c r="N26" s="175"/>
-      <c r="O26" s="175"/>
-      <c r="P26" s="175"/>
-      <c r="Q26" s="175"/>
-      <c r="R26" s="175"/>
-      <c r="S26" s="175"/>
-      <c r="T26" s="180"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="143"/>
-      <c r="B27" s="144"/>
-      <c r="C27" s="144"/>
-      <c r="D27" s="145"/>
-      <c r="E27" s="189"/>
-      <c r="F27" s="184"/>
-      <c r="G27" s="175"/>
-      <c r="H27" s="175"/>
-      <c r="I27" s="176"/>
-      <c r="J27" s="174"/>
-      <c r="K27" s="175"/>
-      <c r="L27" s="176"/>
-      <c r="M27" s="174"/>
-      <c r="N27" s="175"/>
-      <c r="O27" s="175"/>
-      <c r="P27" s="175"/>
-      <c r="Q27" s="175"/>
-      <c r="R27" s="175"/>
-      <c r="S27" s="175"/>
-      <c r="T27" s="180"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="143"/>
-      <c r="B28" s="144"/>
-      <c r="C28" s="144"/>
-      <c r="D28" s="145"/>
-      <c r="E28" s="189"/>
-      <c r="F28" s="184"/>
-      <c r="G28" s="175"/>
-      <c r="H28" s="175"/>
-      <c r="I28" s="176"/>
-      <c r="J28" s="174"/>
-      <c r="K28" s="175"/>
-      <c r="L28" s="176"/>
-      <c r="M28" s="174"/>
-      <c r="N28" s="175"/>
-      <c r="O28" s="175"/>
-      <c r="P28" s="175"/>
-      <c r="Q28" s="175"/>
-      <c r="R28" s="175"/>
-      <c r="S28" s="175"/>
-      <c r="T28" s="180"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="143"/>
-      <c r="B29" s="144"/>
-      <c r="C29" s="144"/>
-      <c r="D29" s="145"/>
-      <c r="E29" s="189"/>
-      <c r="F29" s="184"/>
-      <c r="G29" s="175"/>
-      <c r="H29" s="175"/>
-      <c r="I29" s="176"/>
-      <c r="J29" s="174"/>
-      <c r="K29" s="175"/>
-      <c r="L29" s="176"/>
-      <c r="M29" s="174"/>
-      <c r="N29" s="175"/>
-      <c r="O29" s="175"/>
-      <c r="P29" s="175"/>
-      <c r="Q29" s="175"/>
-      <c r="R29" s="175"/>
-      <c r="S29" s="175"/>
-      <c r="T29" s="180"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="143"/>
-      <c r="B30" s="144"/>
-      <c r="C30" s="144"/>
-      <c r="D30" s="145"/>
-      <c r="E30" s="189"/>
-      <c r="F30" s="184"/>
-      <c r="G30" s="175"/>
-      <c r="H30" s="175"/>
-      <c r="I30" s="176"/>
-      <c r="J30" s="174"/>
-      <c r="K30" s="175"/>
-      <c r="L30" s="176"/>
-      <c r="M30" s="174"/>
-      <c r="N30" s="175"/>
-      <c r="O30" s="175"/>
-      <c r="P30" s="175"/>
-      <c r="Q30" s="175"/>
-      <c r="R30" s="175"/>
-      <c r="S30" s="175"/>
-      <c r="T30" s="180"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="143"/>
-      <c r="B31" s="144"/>
-      <c r="C31" s="144"/>
-      <c r="D31" s="145"/>
-      <c r="E31" s="189"/>
-      <c r="F31" s="184"/>
-      <c r="G31" s="175"/>
-      <c r="H31" s="175"/>
-      <c r="I31" s="176"/>
-      <c r="J31" s="174"/>
-      <c r="K31" s="175"/>
-      <c r="L31" s="176"/>
-      <c r="M31" s="174"/>
-      <c r="N31" s="175"/>
-      <c r="O31" s="175"/>
-      <c r="P31" s="175"/>
-      <c r="Q31" s="175"/>
-      <c r="R31" s="175"/>
-      <c r="S31" s="175"/>
-      <c r="T31" s="180"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="143"/>
-      <c r="B32" s="144"/>
-      <c r="C32" s="144"/>
-      <c r="D32" s="145"/>
-      <c r="E32" s="189"/>
-      <c r="F32" s="184"/>
-      <c r="G32" s="175"/>
-      <c r="H32" s="175"/>
-      <c r="I32" s="176"/>
-      <c r="J32" s="174"/>
-      <c r="K32" s="175"/>
-      <c r="L32" s="176"/>
-      <c r="M32" s="174"/>
-      <c r="N32" s="175"/>
-      <c r="O32" s="175"/>
-      <c r="P32" s="175"/>
-      <c r="Q32" s="175"/>
-      <c r="R32" s="175"/>
-      <c r="S32" s="175"/>
-      <c r="T32" s="180"/>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="171"/>
+      <c r="B20" s="172"/>
+      <c r="C20" s="172"/>
+      <c r="D20" s="173"/>
+      <c r="E20" s="178"/>
+      <c r="F20" s="170"/>
+      <c r="G20" s="158"/>
+      <c r="H20" s="158"/>
+      <c r="I20" s="159"/>
+      <c r="J20" s="157"/>
+      <c r="K20" s="158"/>
+      <c r="L20" s="159"/>
+      <c r="M20" s="157"/>
+      <c r="N20" s="158"/>
+      <c r="O20" s="158"/>
+      <c r="P20" s="158"/>
+      <c r="Q20" s="158"/>
+      <c r="R20" s="158"/>
+      <c r="S20" s="158"/>
+      <c r="T20" s="163"/>
+      <c r="W20" s="87" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="171"/>
+      <c r="B21" s="172"/>
+      <c r="C21" s="172"/>
+      <c r="D21" s="173"/>
+      <c r="E21" s="178"/>
+      <c r="F21" s="170"/>
+      <c r="G21" s="158"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="159"/>
+      <c r="J21" s="157"/>
+      <c r="K21" s="158"/>
+      <c r="L21" s="159"/>
+      <c r="M21" s="157"/>
+      <c r="N21" s="158"/>
+      <c r="O21" s="158"/>
+      <c r="P21" s="158"/>
+      <c r="Q21" s="158"/>
+      <c r="R21" s="158"/>
+      <c r="S21" s="158"/>
+      <c r="T21" s="163"/>
+      <c r="W21" s="87" t="s">
+        <v>58</v>
+      </c>
+      <c r="X21" s="87" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y21" s="88" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="171"/>
+      <c r="B22" s="172"/>
+      <c r="C22" s="172"/>
+      <c r="D22" s="173"/>
+      <c r="E22" s="178"/>
+      <c r="F22" s="170"/>
+      <c r="G22" s="158"/>
+      <c r="H22" s="158"/>
+      <c r="I22" s="159"/>
+      <c r="J22" s="157"/>
+      <c r="K22" s="158"/>
+      <c r="L22" s="159"/>
+      <c r="M22" s="157"/>
+      <c r="N22" s="158"/>
+      <c r="O22" s="158"/>
+      <c r="P22" s="158"/>
+      <c r="Q22" s="158"/>
+      <c r="R22" s="158"/>
+      <c r="S22" s="158"/>
+      <c r="T22" s="163"/>
+      <c r="W22" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="X22" s="87" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y22" s="87" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="171"/>
+      <c r="B23" s="172"/>
+      <c r="C23" s="172"/>
+      <c r="D23" s="173"/>
+      <c r="E23" s="178"/>
+      <c r="F23" s="170"/>
+      <c r="G23" s="158"/>
+      <c r="H23" s="158"/>
+      <c r="I23" s="159"/>
+      <c r="J23" s="157"/>
+      <c r="K23" s="158"/>
+      <c r="L23" s="159"/>
+      <c r="M23" s="157"/>
+      <c r="N23" s="158"/>
+      <c r="O23" s="158"/>
+      <c r="P23" s="158"/>
+      <c r="Q23" s="158"/>
+      <c r="R23" s="158"/>
+      <c r="S23" s="158"/>
+      <c r="T23" s="163"/>
+      <c r="W23" s="88" t="s">
+        <v>226</v>
+      </c>
+      <c r="X23" s="87" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" s="171"/>
+      <c r="B24" s="172"/>
+      <c r="C24" s="172"/>
+      <c r="D24" s="173"/>
+      <c r="E24" s="178"/>
+      <c r="F24" s="170"/>
+      <c r="G24" s="158"/>
+      <c r="H24" s="158"/>
+      <c r="I24" s="159"/>
+      <c r="J24" s="157"/>
+      <c r="K24" s="158"/>
+      <c r="L24" s="159"/>
+      <c r="M24" s="157"/>
+      <c r="N24" s="158"/>
+      <c r="O24" s="158"/>
+      <c r="P24" s="158"/>
+      <c r="Q24" s="158"/>
+      <c r="R24" s="158"/>
+      <c r="S24" s="158"/>
+      <c r="T24" s="163"/>
+      <c r="W24" s="88" t="s">
+        <v>227</v>
+      </c>
+      <c r="X24" s="87" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="171"/>
+      <c r="B25" s="172"/>
+      <c r="C25" s="172"/>
+      <c r="D25" s="173"/>
+      <c r="E25" s="178"/>
+      <c r="F25" s="170"/>
+      <c r="G25" s="158"/>
+      <c r="H25" s="158"/>
+      <c r="I25" s="159"/>
+      <c r="J25" s="157"/>
+      <c r="K25" s="158"/>
+      <c r="L25" s="159"/>
+      <c r="M25" s="157"/>
+      <c r="N25" s="158"/>
+      <c r="O25" s="158"/>
+      <c r="P25" s="158"/>
+      <c r="Q25" s="158"/>
+      <c r="R25" s="158"/>
+      <c r="S25" s="158"/>
+      <c r="T25" s="163"/>
+      <c r="W25" s="88" t="s">
+        <v>228</v>
+      </c>
+      <c r="X25" s="87" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="171"/>
+      <c r="B26" s="172"/>
+      <c r="C26" s="172"/>
+      <c r="D26" s="173"/>
+      <c r="E26" s="178"/>
+      <c r="F26" s="170"/>
+      <c r="G26" s="158"/>
+      <c r="H26" s="158"/>
+      <c r="I26" s="159"/>
+      <c r="J26" s="157"/>
+      <c r="K26" s="158"/>
+      <c r="L26" s="159"/>
+      <c r="M26" s="157"/>
+      <c r="N26" s="158"/>
+      <c r="O26" s="158"/>
+      <c r="P26" s="158"/>
+      <c r="Q26" s="158"/>
+      <c r="R26" s="158"/>
+      <c r="S26" s="158"/>
+      <c r="T26" s="163"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" s="171"/>
+      <c r="B27" s="172"/>
+      <c r="C27" s="172"/>
+      <c r="D27" s="173"/>
+      <c r="E27" s="178"/>
+      <c r="F27" s="170"/>
+      <c r="G27" s="158"/>
+      <c r="H27" s="158"/>
+      <c r="I27" s="159"/>
+      <c r="J27" s="157"/>
+      <c r="K27" s="158"/>
+      <c r="L27" s="159"/>
+      <c r="M27" s="157"/>
+      <c r="N27" s="158"/>
+      <c r="O27" s="158"/>
+      <c r="P27" s="158"/>
+      <c r="Q27" s="158"/>
+      <c r="R27" s="158"/>
+      <c r="S27" s="158"/>
+      <c r="T27" s="163"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="171"/>
+      <c r="B28" s="172"/>
+      <c r="C28" s="172"/>
+      <c r="D28" s="173"/>
+      <c r="E28" s="178"/>
+      <c r="F28" s="170"/>
+      <c r="G28" s="158"/>
+      <c r="H28" s="158"/>
+      <c r="I28" s="159"/>
+      <c r="J28" s="157"/>
+      <c r="K28" s="158"/>
+      <c r="L28" s="159"/>
+      <c r="M28" s="157"/>
+      <c r="N28" s="158"/>
+      <c r="O28" s="158"/>
+      <c r="P28" s="158"/>
+      <c r="Q28" s="158"/>
+      <c r="R28" s="158"/>
+      <c r="S28" s="158"/>
+      <c r="T28" s="163"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="171"/>
+      <c r="B29" s="172"/>
+      <c r="C29" s="172"/>
+      <c r="D29" s="173"/>
+      <c r="E29" s="178"/>
+      <c r="F29" s="170"/>
+      <c r="G29" s="158"/>
+      <c r="H29" s="158"/>
+      <c r="I29" s="159"/>
+      <c r="J29" s="157"/>
+      <c r="K29" s="158"/>
+      <c r="L29" s="159"/>
+      <c r="M29" s="157"/>
+      <c r="N29" s="158"/>
+      <c r="O29" s="158"/>
+      <c r="P29" s="158"/>
+      <c r="Q29" s="158"/>
+      <c r="R29" s="158"/>
+      <c r="S29" s="158"/>
+      <c r="T29" s="163"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="171"/>
+      <c r="B30" s="172"/>
+      <c r="C30" s="172"/>
+      <c r="D30" s="173"/>
+      <c r="E30" s="178"/>
+      <c r="F30" s="170"/>
+      <c r="G30" s="158"/>
+      <c r="H30" s="158"/>
+      <c r="I30" s="159"/>
+      <c r="J30" s="157"/>
+      <c r="K30" s="158"/>
+      <c r="L30" s="159"/>
+      <c r="M30" s="157"/>
+      <c r="N30" s="158"/>
+      <c r="O30" s="158"/>
+      <c r="P30" s="158"/>
+      <c r="Q30" s="158"/>
+      <c r="R30" s="158"/>
+      <c r="S30" s="158"/>
+      <c r="T30" s="163"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" s="171"/>
+      <c r="B31" s="172"/>
+      <c r="C31" s="172"/>
+      <c r="D31" s="173"/>
+      <c r="E31" s="178"/>
+      <c r="F31" s="170"/>
+      <c r="G31" s="158"/>
+      <c r="H31" s="158"/>
+      <c r="I31" s="159"/>
+      <c r="J31" s="157"/>
+      <c r="K31" s="158"/>
+      <c r="L31" s="159"/>
+      <c r="M31" s="157"/>
+      <c r="N31" s="158"/>
+      <c r="O31" s="158"/>
+      <c r="P31" s="158"/>
+      <c r="Q31" s="158"/>
+      <c r="R31" s="158"/>
+      <c r="S31" s="158"/>
+      <c r="T31" s="163"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="171"/>
+      <c r="B32" s="172"/>
+      <c r="C32" s="172"/>
+      <c r="D32" s="173"/>
+      <c r="E32" s="178"/>
+      <c r="F32" s="170"/>
+      <c r="G32" s="158"/>
+      <c r="H32" s="158"/>
+      <c r="I32" s="159"/>
+      <c r="J32" s="157"/>
+      <c r="K32" s="158"/>
+      <c r="L32" s="159"/>
+      <c r="M32" s="157"/>
+      <c r="N32" s="158"/>
+      <c r="O32" s="158"/>
+      <c r="P32" s="158"/>
+      <c r="Q32" s="158"/>
+      <c r="R32" s="158"/>
+      <c r="S32" s="158"/>
+      <c r="T32" s="163"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="143"/>
-      <c r="B33" s="144"/>
-      <c r="C33" s="144"/>
-      <c r="D33" s="145"/>
-      <c r="E33" s="189"/>
-      <c r="F33" s="184"/>
-      <c r="G33" s="175"/>
-      <c r="H33" s="175"/>
-      <c r="I33" s="176"/>
-      <c r="J33" s="174"/>
-      <c r="K33" s="175"/>
-      <c r="L33" s="176"/>
-      <c r="M33" s="174"/>
-      <c r="N33" s="175"/>
-      <c r="O33" s="175"/>
-      <c r="P33" s="175"/>
-      <c r="Q33" s="175"/>
-      <c r="R33" s="175"/>
-      <c r="S33" s="175"/>
-      <c r="T33" s="180"/>
+      <c r="A33" s="171"/>
+      <c r="B33" s="172"/>
+      <c r="C33" s="172"/>
+      <c r="D33" s="173"/>
+      <c r="E33" s="178"/>
+      <c r="F33" s="170"/>
+      <c r="G33" s="158"/>
+      <c r="H33" s="158"/>
+      <c r="I33" s="159"/>
+      <c r="J33" s="157"/>
+      <c r="K33" s="158"/>
+      <c r="L33" s="159"/>
+      <c r="M33" s="157"/>
+      <c r="N33" s="158"/>
+      <c r="O33" s="158"/>
+      <c r="P33" s="158"/>
+      <c r="Q33" s="158"/>
+      <c r="R33" s="158"/>
+      <c r="S33" s="158"/>
+      <c r="T33" s="163"/>
     </row>
     <row r="34" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="185"/>
-      <c r="B34" s="186"/>
-      <c r="C34" s="186"/>
-      <c r="D34" s="187"/>
-      <c r="E34" s="190"/>
-      <c r="F34" s="191"/>
-      <c r="G34" s="178"/>
-      <c r="H34" s="178"/>
-      <c r="I34" s="179"/>
-      <c r="J34" s="177"/>
-      <c r="K34" s="178"/>
-      <c r="L34" s="179"/>
-      <c r="M34" s="177"/>
-      <c r="N34" s="178"/>
-      <c r="O34" s="178"/>
-      <c r="P34" s="178"/>
-      <c r="Q34" s="178"/>
-      <c r="R34" s="178"/>
-      <c r="S34" s="178"/>
-      <c r="T34" s="181"/>
+      <c r="A34" s="174"/>
+      <c r="B34" s="175"/>
+      <c r="C34" s="175"/>
+      <c r="D34" s="176"/>
+      <c r="E34" s="179"/>
+      <c r="F34" s="180"/>
+      <c r="G34" s="161"/>
+      <c r="H34" s="161"/>
+      <c r="I34" s="162"/>
+      <c r="J34" s="160"/>
+      <c r="K34" s="161"/>
+      <c r="L34" s="162"/>
+      <c r="M34" s="160"/>
+      <c r="N34" s="161"/>
+      <c r="O34" s="161"/>
+      <c r="P34" s="161"/>
+      <c r="Q34" s="161"/>
+      <c r="R34" s="161"/>
+      <c r="S34" s="161"/>
+      <c r="T34" s="164"/>
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="A13:D14"/>
+    <mergeCell ref="A15:D18"/>
+    <mergeCell ref="A7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="M7:T8"/>
+    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="M5:P5"/>
+    <mergeCell ref="Q5:T5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="I7:L8"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="Q3:T3"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="M11:T12"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="J19:L34"/>
+    <mergeCell ref="M19:T34"/>
+    <mergeCell ref="K9:T9"/>
+    <mergeCell ref="J10:T10"/>
+    <mergeCell ref="M13:T14"/>
+    <mergeCell ref="I13:L14"/>
+    <mergeCell ref="L15:N18"/>
+    <mergeCell ref="O15:Q18"/>
+    <mergeCell ref="R15:T18"/>
+    <mergeCell ref="H15:K18"/>
+    <mergeCell ref="A19:D34"/>
+    <mergeCell ref="E19:E34"/>
+    <mergeCell ref="F19:I34"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="C6:D6"/>
@@ -5698,48 +6075,6 @@
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="H11:H12"/>
-    <mergeCell ref="M11:T12"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="J19:L34"/>
-    <mergeCell ref="M19:T34"/>
-    <mergeCell ref="K9:T9"/>
-    <mergeCell ref="J10:T10"/>
-    <mergeCell ref="M13:T14"/>
-    <mergeCell ref="I13:L14"/>
-    <mergeCell ref="L15:N18"/>
-    <mergeCell ref="O15:Q18"/>
-    <mergeCell ref="R15:T18"/>
-    <mergeCell ref="H15:K18"/>
-    <mergeCell ref="A19:D34"/>
-    <mergeCell ref="E19:E34"/>
-    <mergeCell ref="F19:I34"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="Q3:T3"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="M7:T8"/>
-    <mergeCell ref="O6:T6"/>
-    <mergeCell ref="M5:P5"/>
-    <mergeCell ref="Q5:T5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="I7:L8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="A13:D14"/>
-    <mergeCell ref="A15:D18"/>
-    <mergeCell ref="A7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6278,8 +6613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6312,16 +6647,16 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="113">
+      <c r="A2" s="108">
         <v>0</v>
       </c>
-      <c r="B2" s="114">
+      <c r="B2" s="109">
         <v>0</v>
       </c>
-      <c r="C2" s="114">
+      <c r="C2" s="109">
         <v>0</v>
       </c>
-      <c r="D2" s="115">
+      <c r="D2" s="110">
         <v>0</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -6335,16 +6670,16 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="116">
+      <c r="A3" s="111">
         <v>0</v>
       </c>
-      <c r="B3" s="117">
+      <c r="B3" s="112">
         <v>0</v>
       </c>
-      <c r="C3" s="117">
+      <c r="C3" s="112">
         <v>0</v>
       </c>
-      <c r="D3" s="118">
+      <c r="D3" s="113">
         <v>1</v>
       </c>
       <c r="E3" s="9" t="s">
@@ -6358,16 +6693,16 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="116">
+      <c r="A4" s="111">
         <v>0</v>
       </c>
-      <c r="B4" s="117">
+      <c r="B4" s="112">
         <v>0</v>
       </c>
-      <c r="C4" s="117">
+      <c r="C4" s="112">
         <v>1</v>
       </c>
-      <c r="D4" s="118">
+      <c r="D4" s="113">
         <v>0</v>
       </c>
       <c r="E4" s="9" t="s">
@@ -6381,16 +6716,16 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="119">
+      <c r="A5" s="114">
         <v>0</v>
       </c>
-      <c r="B5" s="120">
+      <c r="B5" s="115">
         <v>0</v>
       </c>
-      <c r="C5" s="120">
+      <c r="C5" s="115">
         <v>1</v>
       </c>
-      <c r="D5" s="121">
+      <c r="D5" s="116">
         <v>1</v>
       </c>
       <c r="E5" s="12" t="s">
@@ -6404,16 +6739,16 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="113">
+      <c r="A6" s="108">
         <v>0</v>
       </c>
-      <c r="B6" s="114">
+      <c r="B6" s="109">
         <v>1</v>
       </c>
-      <c r="C6" s="114">
+      <c r="C6" s="109">
         <v>0</v>
       </c>
-      <c r="D6" s="115">
+      <c r="D6" s="110">
         <v>0</v>
       </c>
       <c r="E6" s="6" t="s">
@@ -6427,16 +6762,16 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="116">
+      <c r="A7" s="111">
         <v>0</v>
       </c>
-      <c r="B7" s="117">
+      <c r="B7" s="112">
         <v>1</v>
       </c>
-      <c r="C7" s="117">
+      <c r="C7" s="112">
         <v>0</v>
       </c>
-      <c r="D7" s="118">
+      <c r="D7" s="113">
         <v>1</v>
       </c>
       <c r="E7" s="11" t="s">
@@ -6450,16 +6785,16 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="116">
+      <c r="A8" s="111">
         <v>0</v>
       </c>
-      <c r="B8" s="117">
+      <c r="B8" s="112">
         <v>1</v>
       </c>
-      <c r="C8" s="117">
+      <c r="C8" s="112">
         <v>1</v>
       </c>
-      <c r="D8" s="118">
+      <c r="D8" s="113">
         <v>0</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -6473,16 +6808,16 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="119">
+      <c r="A9" s="114">
         <v>0</v>
       </c>
-      <c r="B9" s="120">
+      <c r="B9" s="115">
         <v>1</v>
       </c>
-      <c r="C9" s="120">
+      <c r="C9" s="115">
         <v>1</v>
       </c>
-      <c r="D9" s="121">
+      <c r="D9" s="116">
         <v>1</v>
       </c>
       <c r="E9" s="12" t="s">
@@ -6496,16 +6831,16 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="113">
+      <c r="A10" s="108">
         <v>1</v>
       </c>
-      <c r="B10" s="114">
+      <c r="B10" s="109">
         <v>0</v>
       </c>
-      <c r="C10" s="114">
+      <c r="C10" s="109">
         <v>0</v>
       </c>
-      <c r="D10" s="115">
+      <c r="D10" s="110">
         <v>0</v>
       </c>
       <c r="E10" s="6" t="s">
@@ -6519,16 +6854,16 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="116">
+      <c r="A11" s="111">
         <v>1</v>
       </c>
-      <c r="B11" s="117">
+      <c r="B11" s="112">
         <v>0</v>
       </c>
-      <c r="C11" s="117">
+      <c r="C11" s="112">
         <v>0</v>
       </c>
-      <c r="D11" s="118">
+      <c r="D11" s="113">
         <v>1</v>
       </c>
       <c r="E11" s="9" t="s">
@@ -6542,16 +6877,16 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="116">
+      <c r="A12" s="111">
         <v>1</v>
       </c>
-      <c r="B12" s="117">
+      <c r="B12" s="112">
         <v>0</v>
       </c>
-      <c r="C12" s="117">
+      <c r="C12" s="112">
         <v>1</v>
       </c>
-      <c r="D12" s="118">
+      <c r="D12" s="113">
         <v>0</v>
       </c>
       <c r="E12" s="9" t="s">
@@ -6565,16 +6900,16 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="119">
+      <c r="A13" s="114">
         <v>1</v>
       </c>
-      <c r="B13" s="120">
+      <c r="B13" s="115">
         <v>0</v>
       </c>
-      <c r="C13" s="120">
+      <c r="C13" s="115">
         <v>1</v>
       </c>
-      <c r="D13" s="121">
+      <c r="D13" s="116">
         <v>1</v>
       </c>
       <c r="E13" s="12" t="s">
@@ -6588,16 +6923,16 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="122">
+      <c r="A14" s="117">
         <v>1</v>
       </c>
-      <c r="B14" s="123">
+      <c r="B14" s="118">
         <v>1</v>
       </c>
-      <c r="C14" s="123">
+      <c r="C14" s="118">
         <v>0</v>
       </c>
-      <c r="D14" s="124">
+      <c r="D14" s="119">
         <v>0</v>
       </c>
       <c r="E14" s="6" t="s">
@@ -6611,16 +6946,16 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="116">
+      <c r="A15" s="111">
         <v>1</v>
       </c>
-      <c r="B15" s="117">
+      <c r="B15" s="112">
         <v>1</v>
       </c>
-      <c r="C15" s="117">
+      <c r="C15" s="112">
         <v>0</v>
       </c>
-      <c r="D15" s="118">
+      <c r="D15" s="113">
         <v>1</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -6634,16 +6969,16 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="116">
+      <c r="A16" s="111">
         <v>1</v>
       </c>
-      <c r="B16" s="117">
+      <c r="B16" s="112">
         <v>1</v>
       </c>
-      <c r="C16" s="117">
+      <c r="C16" s="112">
         <v>1</v>
       </c>
-      <c r="D16" s="118">
+      <c r="D16" s="113">
         <v>0</v>
       </c>
       <c r="E16" s="9" t="s">
@@ -6657,16 +6992,16 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="119">
+      <c r="A17" s="114">
         <v>1</v>
       </c>
-      <c r="B17" s="120">
+      <c r="B17" s="115">
         <v>1</v>
       </c>
-      <c r="C17" s="120">
+      <c r="C17" s="115">
         <v>1</v>
       </c>
-      <c r="D17" s="121">
+      <c r="D17" s="116">
         <v>1</v>
       </c>
       <c r="E17" s="12" t="s">

</xml_diff>

<commit_message>
Hardware implementation of Register Files
New Vivado project is created,
GPR and ADR files are created up to spec
</commit_message>
<xml_diff>
--- a/Instruction Set/InstSet.xlsx
+++ b/Instruction Set/InstSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cemal\Documents\GitHub\myCPU\Instruction Set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EA0589-829D-4C8C-A995-FCD90AFB1D60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7819E4ED-1156-4FD7-903B-EFB23B7C0F47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Decoder" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="301">
   <si>
     <t>S3</t>
   </si>
@@ -676,9 +676,6 @@
     <t>ADR C + GPR C</t>
   </si>
   <si>
-    <t>sc[4]</t>
-  </si>
-  <si>
     <t>ADR C + Imm6</t>
   </si>
   <si>
@@ -929,6 +926,12 @@
   </si>
   <si>
     <t>VC</t>
+  </si>
+  <si>
+    <t>sc[2]</t>
+  </si>
+  <si>
+    <t>sc[3]</t>
   </si>
 </sst>
 </file>
@@ -2261,6 +2264,192 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="57" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="29" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="58" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="27" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="30" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="44" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="46" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="40" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="33" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="38" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="37" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2270,67 +2459,13 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="57" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="29" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="58" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="27" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="40" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="33" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="46" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2341,138 +2476,6 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="30" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="44" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="38" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="37" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3098,7 +3101,7 @@
     </row>
     <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B10" s="30" t="s">
         <v>92</v>
@@ -3150,7 +3153,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B12" s="58"/>
       <c r="C12" s="59"/>
@@ -3190,14 +3193,14 @@
         <v>67</v>
       </c>
       <c r="H13" s="63" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I13" s="43"/>
       <c r="O13" s="17"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B14" s="58" t="s">
         <v>87</v>
@@ -3229,7 +3232,7 @@
         <v>87</v>
       </c>
       <c r="C15" s="62" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D15" s="62" t="s">
         <v>99</v>
@@ -3372,7 +3375,7 @@
         <v>92</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -3386,7 +3389,7 @@
         <v>86</v>
       </c>
       <c r="I21" s="43" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3411,7 +3414,7 @@
         <v>86</v>
       </c>
       <c r="I22" s="23" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3422,7 +3425,7 @@
         <v>106</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
@@ -3436,7 +3439,7 @@
         <v>49</v>
       </c>
       <c r="I23" s="37" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3447,7 +3450,7 @@
         <v>106</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
@@ -3461,13 +3464,13 @@
         <v>80</v>
       </c>
       <c r="I24" s="37" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J24" s="40"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="42" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>175</v>
@@ -3487,18 +3490,18 @@
         <v>86</v>
       </c>
       <c r="I25" s="37" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="42" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B26" s="20" t="s">
         <v>175</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
@@ -3509,7 +3512,7 @@
         <v>67</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -3530,7 +3533,7 @@
         <v>49</v>
       </c>
       <c r="I27" s="43" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3568,7 +3571,7 @@
         <v>80</v>
       </c>
       <c r="I29" s="37" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3590,7 +3593,7 @@
     </row>
     <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="48" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B31" t="s">
         <v>175</v>
@@ -3711,8 +3714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9489E50B-F7AE-40DA-B3EF-ED84A344FCCC}">
   <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:U6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3833,7 +3836,7 @@
         <v>162</v>
       </c>
       <c r="N3" s="46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P3" s="46">
         <v>1</v>
@@ -3843,13 +3846,13 @@
       </c>
       <c r="R3" s="47"/>
       <c r="S3" s="88" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T3" s="87" t="s">
         <v>57</v>
       </c>
       <c r="U3" s="87" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -3880,7 +3883,7 @@
       </c>
       <c r="R4" s="47"/>
       <c r="S4" s="88" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T4" s="87" t="s">
         <v>55</v>
@@ -3922,7 +3925,7 @@
       </c>
       <c r="R5" s="47"/>
       <c r="S5" s="88" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="T5" s="87" t="s">
         <v>54</v>
@@ -3966,7 +3969,7 @@
         <v>144</v>
       </c>
       <c r="S6" s="88" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="T6" s="87" t="s">
         <v>56</v>
@@ -4011,7 +4014,7 @@
         <v>105</v>
       </c>
       <c r="B8" s="53" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C8" s="80" t="s">
         <v>161</v>
@@ -4221,7 +4224,7 @@
         <v>162</v>
       </c>
       <c r="N13" s="46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P13" s="46" t="s">
         <v>162</v>
@@ -4295,16 +4298,16 @@
     </row>
     <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="55" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D18" s="57" t="s">
         <v>201</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F18" s="56" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G18" s="57" t="s">
         <v>153</v>
@@ -4449,15 +4452,15 @@
         <v>166</v>
       </c>
       <c r="N22" s="46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="52" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B23" s="53" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C23" s="78" t="s">
         <v>189</v>
@@ -4511,14 +4514,14 @@
         <v>173</v>
       </c>
       <c r="B25" s="53" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C25" s="78" t="s">
         <v>205</v>
       </c>
       <c r="D25" s="83"/>
       <c r="E25" s="78" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F25" s="79" t="s">
         <v>162</v>
@@ -4539,14 +4542,14 @@
         <v>173</v>
       </c>
       <c r="B26" s="56" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C26" s="75" t="s">
         <v>205</v>
       </c>
       <c r="D26" s="76"/>
       <c r="E26" s="75" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F26" s="77" t="s">
         <v>162</v>
@@ -4588,10 +4591,10 @@
     </row>
     <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="65" t="s">
-        <v>215</v>
+        <v>300</v>
       </c>
       <c r="D30" s="65" t="s">
-        <v>215</v>
+        <v>299</v>
       </c>
       <c r="E30" s="54" t="s">
         <v>211</v>
@@ -4694,7 +4697,7 @@
     </row>
     <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="52" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D41" s="54" t="s">
         <v>201</v>
@@ -4717,10 +4720,10 @@
         <v>90</v>
       </c>
       <c r="B43" s="53" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C43" s="78" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D43" s="83" t="s">
         <v>149</v>
@@ -4731,10 +4734,10 @@
         <v>100</v>
       </c>
       <c r="B44" s="53" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C44" s="78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D44" s="83" t="s">
         <v>149</v>
@@ -4745,10 +4748,10 @@
         <v>98</v>
       </c>
       <c r="B45" s="56" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C45" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D45" s="76" t="s">
         <v>150</v>
@@ -4774,7 +4777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F660B940-324A-409A-9742-8BFC9B3A5F3A}">
   <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X21" sqref="X21:X22"/>
     </sheetView>
   </sheetViews>
@@ -4787,12 +4790,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="187" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="127"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="189"/>
       <c r="E1" s="91">
         <v>15</v>
       </c>
@@ -4844,16 +4847,16 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="95" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" s="96" t="s">
         <v>237</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="C2" s="96" t="s">
         <v>238</v>
       </c>
-      <c r="C2" s="96" t="s">
+      <c r="D2" s="97" t="s">
         <v>239</v>
-      </c>
-      <c r="D2" s="97" t="s">
-        <v>240</v>
       </c>
       <c r="E2" s="98">
         <v>0</v>
@@ -4870,23 +4873,23 @@
       <c r="I2" s="100">
         <v>0</v>
       </c>
-      <c r="J2" s="192" t="s">
+      <c r="J2" s="125" t="s">
         <v>123</v>
       </c>
-      <c r="K2" s="193"/>
-      <c r="L2" s="194"/>
-      <c r="M2" s="167" t="s">
+      <c r="K2" s="126"/>
+      <c r="L2" s="127"/>
+      <c r="M2" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="168"/>
-      <c r="O2" s="168"/>
-      <c r="P2" s="168"/>
-      <c r="Q2" s="168" t="s">
+      <c r="N2" s="182"/>
+      <c r="O2" s="182"/>
+      <c r="P2" s="182"/>
+      <c r="Q2" s="182" t="s">
         <v>124</v>
       </c>
-      <c r="R2" s="168"/>
-      <c r="S2" s="168"/>
-      <c r="T2" s="169"/>
+      <c r="R2" s="182"/>
+      <c r="S2" s="182"/>
+      <c r="T2" s="183"/>
       <c r="V2" s="87" t="s">
         <v>81</v>
       </c>
@@ -4922,31 +4925,31 @@
       <c r="I3" s="105">
         <v>1</v>
       </c>
-      <c r="J3" s="170" t="s">
+      <c r="J3" s="128" t="s">
         <v>123</v>
       </c>
-      <c r="K3" s="170"/>
-      <c r="L3" s="195"/>
-      <c r="M3" s="161" t="s">
+      <c r="K3" s="128"/>
+      <c r="L3" s="129"/>
+      <c r="M3" s="184" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="170"/>
-      <c r="O3" s="170"/>
-      <c r="P3" s="170"/>
-      <c r="Q3" s="170" t="s">
+      <c r="N3" s="128"/>
+      <c r="O3" s="128"/>
+      <c r="P3" s="128"/>
+      <c r="Q3" s="128" t="s">
         <v>124</v>
       </c>
-      <c r="R3" s="170"/>
-      <c r="S3" s="170"/>
-      <c r="T3" s="171"/>
+      <c r="R3" s="128"/>
+      <c r="S3" s="128"/>
+      <c r="T3" s="185"/>
       <c r="V3" s="87" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="W3" s="87" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Y3" s="87" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Z3" s="87" t="s">
         <v>8</v>
@@ -4956,11 +4959,11 @@
       <c r="A4" s="107" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="146" t="s">
+      <c r="B4" s="130" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="147"/>
-      <c r="D4" s="148"/>
+      <c r="C4" s="152"/>
+      <c r="D4" s="131"/>
       <c r="E4" s="104">
         <v>0</v>
       </c>
@@ -4979,42 +4982,42 @@
       <c r="J4" s="120">
         <v>0</v>
       </c>
-      <c r="K4" s="170" t="s">
+      <c r="K4" s="128" t="s">
         <v>123</v>
       </c>
-      <c r="L4" s="195"/>
-      <c r="M4" s="161" t="s">
+      <c r="L4" s="129"/>
+      <c r="M4" s="184" t="s">
         <v>122</v>
       </c>
-      <c r="N4" s="170"/>
-      <c r="O4" s="170"/>
-      <c r="P4" s="170"/>
-      <c r="Q4" s="170" t="s">
+      <c r="N4" s="128"/>
+      <c r="O4" s="128"/>
+      <c r="P4" s="128"/>
+      <c r="Q4" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="R4" s="170"/>
-      <c r="S4" s="170"/>
-      <c r="T4" s="171"/>
+      <c r="R4" s="128"/>
+      <c r="S4" s="128"/>
+      <c r="T4" s="185"/>
       <c r="V4" s="87" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="W4" s="87" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Y4" s="87" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Z4" s="87" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="149" t="s">
-        <v>243</v>
-      </c>
-      <c r="B5" s="150"/>
-      <c r="C5" s="150"/>
-      <c r="D5" s="151"/>
+      <c r="A5" s="193" t="s">
+        <v>242</v>
+      </c>
+      <c r="B5" s="194"/>
+      <c r="C5" s="194"/>
+      <c r="D5" s="195"/>
       <c r="E5" s="104">
         <v>0</v>
       </c>
@@ -5033,44 +5036,44 @@
       <c r="J5" s="124">
         <v>1</v>
       </c>
-      <c r="K5" s="162" t="s">
+      <c r="K5" s="165" t="s">
         <v>171</v>
       </c>
-      <c r="L5" s="161"/>
-      <c r="M5" s="158" t="s">
+      <c r="L5" s="184"/>
+      <c r="M5" s="186" t="s">
         <v>124</v>
       </c>
-      <c r="N5" s="159"/>
-      <c r="O5" s="159"/>
-      <c r="P5" s="161"/>
-      <c r="Q5" s="158" t="s">
+      <c r="N5" s="166"/>
+      <c r="O5" s="166"/>
+      <c r="P5" s="184"/>
+      <c r="Q5" s="186" t="s">
         <v>172</v>
       </c>
-      <c r="R5" s="159"/>
-      <c r="S5" s="159"/>
-      <c r="T5" s="160"/>
+      <c r="R5" s="166"/>
+      <c r="S5" s="166"/>
+      <c r="T5" s="167"/>
       <c r="V5" s="87" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="W5" s="87" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Y5" s="87" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Z5" s="87" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="172" t="s">
+      <c r="A6" s="150" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="173"/>
-      <c r="C6" s="146" t="s">
+      <c r="B6" s="151"/>
+      <c r="C6" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="148"/>
+      <c r="D6" s="131"/>
       <c r="E6" s="104">
         <v>0</v>
       </c>
@@ -5089,124 +5092,124 @@
       <c r="J6" s="124" t="s">
         <v>123</v>
       </c>
-      <c r="K6" s="162" t="s">
+      <c r="K6" s="165" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="159"/>
-      <c r="M6" s="159"/>
-      <c r="N6" s="161"/>
-      <c r="O6" s="158" t="s">
+      <c r="L6" s="166"/>
+      <c r="M6" s="166"/>
+      <c r="N6" s="184"/>
+      <c r="O6" s="186" t="s">
         <v>130</v>
       </c>
-      <c r="P6" s="159"/>
-      <c r="Q6" s="159"/>
-      <c r="R6" s="159"/>
-      <c r="S6" s="159"/>
-      <c r="T6" s="160"/>
+      <c r="P6" s="166"/>
+      <c r="Q6" s="166"/>
+      <c r="R6" s="166"/>
+      <c r="S6" s="166"/>
+      <c r="T6" s="167"/>
       <c r="V6" s="87" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="W6" s="87" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="Y6" s="87" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Z6" s="87" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="137" t="s">
+      <c r="A7" s="136" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="138"/>
-      <c r="C7" s="138"/>
-      <c r="D7" s="139"/>
+      <c r="B7" s="137"/>
+      <c r="C7" s="137"/>
+      <c r="D7" s="138"/>
       <c r="E7" s="134">
         <v>0</v>
       </c>
-      <c r="F7" s="131">
+      <c r="F7" s="132">
         <v>0</v>
       </c>
-      <c r="G7" s="131">
+      <c r="G7" s="132">
         <v>1</v>
       </c>
-      <c r="H7" s="128">
+      <c r="H7" s="148">
         <v>0</v>
       </c>
-      <c r="I7" s="163" t="s">
+      <c r="I7" s="142" t="s">
         <v>122</v>
       </c>
-      <c r="J7" s="153"/>
-      <c r="K7" s="153"/>
-      <c r="L7" s="164"/>
-      <c r="M7" s="152" t="s">
+      <c r="J7" s="143"/>
+      <c r="K7" s="143"/>
+      <c r="L7" s="144"/>
+      <c r="M7" s="153" t="s">
         <v>129</v>
       </c>
-      <c r="N7" s="153"/>
-      <c r="O7" s="153"/>
-      <c r="P7" s="153"/>
-      <c r="Q7" s="153"/>
-      <c r="R7" s="153"/>
-      <c r="S7" s="153"/>
+      <c r="N7" s="143"/>
+      <c r="O7" s="143"/>
+      <c r="P7" s="143"/>
+      <c r="Q7" s="143"/>
+      <c r="R7" s="143"/>
+      <c r="S7" s="143"/>
       <c r="T7" s="154"/>
       <c r="V7" s="87" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="W7" s="87" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Y7" s="87" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Z7" s="87" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="140"/>
-      <c r="B8" s="141"/>
-      <c r="C8" s="141"/>
-      <c r="D8" s="142"/>
-      <c r="E8" s="136"/>
+      <c r="A8" s="139"/>
+      <c r="B8" s="140"/>
+      <c r="C8" s="140"/>
+      <c r="D8" s="141"/>
+      <c r="E8" s="135"/>
       <c r="F8" s="133"/>
       <c r="G8" s="133"/>
-      <c r="H8" s="130"/>
-      <c r="I8" s="165"/>
-      <c r="J8" s="156"/>
-      <c r="K8" s="156"/>
-      <c r="L8" s="166"/>
+      <c r="H8" s="149"/>
+      <c r="I8" s="145"/>
+      <c r="J8" s="146"/>
+      <c r="K8" s="146"/>
+      <c r="L8" s="147"/>
       <c r="M8" s="155"/>
-      <c r="N8" s="156"/>
-      <c r="O8" s="156"/>
-      <c r="P8" s="156"/>
-      <c r="Q8" s="156"/>
-      <c r="R8" s="156"/>
-      <c r="S8" s="156"/>
-      <c r="T8" s="157"/>
+      <c r="N8" s="146"/>
+      <c r="O8" s="146"/>
+      <c r="P8" s="146"/>
+      <c r="Q8" s="146"/>
+      <c r="R8" s="146"/>
+      <c r="S8" s="146"/>
+      <c r="T8" s="156"/>
       <c r="V8" s="87" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="W8" s="87" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Y8" s="87" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Z8" s="87" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="172" t="s">
+      <c r="A9" s="150" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="173"/>
-      <c r="C9" s="146" t="s">
+      <c r="B9" s="151"/>
+      <c r="C9" s="130" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="148"/>
+      <c r="D9" s="131"/>
       <c r="E9" s="104">
         <v>0</v>
       </c>
@@ -5225,38 +5228,38 @@
       <c r="J9" s="124" t="s">
         <v>123</v>
       </c>
-      <c r="K9" s="162" t="s">
+      <c r="K9" s="165" t="s">
         <v>131</v>
       </c>
-      <c r="L9" s="159"/>
-      <c r="M9" s="159"/>
-      <c r="N9" s="159"/>
-      <c r="O9" s="159"/>
-      <c r="P9" s="159"/>
-      <c r="Q9" s="159"/>
-      <c r="R9" s="159"/>
-      <c r="S9" s="159"/>
-      <c r="T9" s="160"/>
+      <c r="L9" s="166"/>
+      <c r="M9" s="166"/>
+      <c r="N9" s="166"/>
+      <c r="O9" s="166"/>
+      <c r="P9" s="166"/>
+      <c r="Q9" s="166"/>
+      <c r="R9" s="166"/>
+      <c r="S9" s="166"/>
+      <c r="T9" s="167"/>
       <c r="V9" s="87" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="W9" s="87" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Y9" s="87" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Z9" s="87" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="172" t="s">
-        <v>231</v>
-      </c>
-      <c r="B10" s="147"/>
-      <c r="C10" s="147"/>
-      <c r="D10" s="148"/>
+      <c r="A10" s="150" t="s">
+        <v>230</v>
+      </c>
+      <c r="B10" s="152"/>
+      <c r="C10" s="152"/>
+      <c r="D10" s="131"/>
       <c r="E10" s="104">
         <v>0</v>
       </c>
@@ -5272,426 +5275,426 @@
       <c r="I10" s="106">
         <v>1</v>
       </c>
-      <c r="J10" s="182" t="s">
+      <c r="J10" s="168" t="s">
         <v>137</v>
       </c>
-      <c r="K10" s="182"/>
-      <c r="L10" s="182"/>
-      <c r="M10" s="182"/>
-      <c r="N10" s="182"/>
-      <c r="O10" s="182"/>
-      <c r="P10" s="182"/>
-      <c r="Q10" s="182"/>
-      <c r="R10" s="182"/>
-      <c r="S10" s="182"/>
-      <c r="T10" s="183"/>
+      <c r="K10" s="168"/>
+      <c r="L10" s="168"/>
+      <c r="M10" s="168"/>
+      <c r="N10" s="168"/>
+      <c r="O10" s="168"/>
+      <c r="P10" s="168"/>
+      <c r="Q10" s="168"/>
+      <c r="R10" s="168"/>
+      <c r="S10" s="168"/>
+      <c r="T10" s="169"/>
       <c r="V10" s="87" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="W10" s="87" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Y10" s="87" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Z10" s="87" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="137" t="s">
+      <c r="A11" s="136" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="138"/>
-      <c r="C11" s="138"/>
-      <c r="D11" s="139"/>
+      <c r="B11" s="137"/>
+      <c r="C11" s="137"/>
+      <c r="D11" s="138"/>
       <c r="E11" s="134">
         <v>0</v>
       </c>
-      <c r="F11" s="131">
+      <c r="F11" s="132">
         <v>1</v>
       </c>
-      <c r="G11" s="131">
+      <c r="G11" s="132">
         <v>0</v>
       </c>
-      <c r="H11" s="128">
+      <c r="H11" s="148">
         <v>0</v>
       </c>
-      <c r="I11" s="163" t="s">
+      <c r="I11" s="142" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="153"/>
-      <c r="K11" s="153"/>
-      <c r="L11" s="164"/>
-      <c r="M11" s="152" t="s">
+      <c r="J11" s="143"/>
+      <c r="K11" s="143"/>
+      <c r="L11" s="144"/>
+      <c r="M11" s="153" t="s">
         <v>129</v>
       </c>
-      <c r="N11" s="153"/>
-      <c r="O11" s="153"/>
-      <c r="P11" s="153"/>
-      <c r="Q11" s="153"/>
-      <c r="R11" s="153"/>
-      <c r="S11" s="153"/>
+      <c r="N11" s="143"/>
+      <c r="O11" s="143"/>
+      <c r="P11" s="143"/>
+      <c r="Q11" s="143"/>
+      <c r="R11" s="143"/>
+      <c r="S11" s="143"/>
       <c r="T11" s="154"/>
       <c r="V11" s="87" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="W11" s="87" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="Y11" s="87" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Z11" s="87" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="140"/>
-      <c r="B12" s="141"/>
-      <c r="C12" s="141"/>
-      <c r="D12" s="142"/>
-      <c r="E12" s="136"/>
+      <c r="A12" s="139"/>
+      <c r="B12" s="140"/>
+      <c r="C12" s="140"/>
+      <c r="D12" s="141"/>
+      <c r="E12" s="135"/>
       <c r="F12" s="133"/>
       <c r="G12" s="133"/>
-      <c r="H12" s="130"/>
-      <c r="I12" s="165"/>
-      <c r="J12" s="156"/>
-      <c r="K12" s="156"/>
-      <c r="L12" s="166"/>
+      <c r="H12" s="149"/>
+      <c r="I12" s="145"/>
+      <c r="J12" s="146"/>
+      <c r="K12" s="146"/>
+      <c r="L12" s="147"/>
       <c r="M12" s="155"/>
-      <c r="N12" s="156"/>
-      <c r="O12" s="156"/>
-      <c r="P12" s="156"/>
-      <c r="Q12" s="156"/>
-      <c r="R12" s="156"/>
-      <c r="S12" s="156"/>
-      <c r="T12" s="157"/>
+      <c r="N12" s="146"/>
+      <c r="O12" s="146"/>
+      <c r="P12" s="146"/>
+      <c r="Q12" s="146"/>
+      <c r="R12" s="146"/>
+      <c r="S12" s="146"/>
+      <c r="T12" s="156"/>
       <c r="V12" s="87" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="W12" s="87" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="Y12" s="87" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Z12" s="87" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="137" t="s">
+      <c r="A13" s="136" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="138"/>
-      <c r="C13" s="138"/>
-      <c r="D13" s="139"/>
+      <c r="B13" s="137"/>
+      <c r="C13" s="137"/>
+      <c r="D13" s="138"/>
       <c r="E13" s="134">
         <v>0</v>
       </c>
-      <c r="F13" s="131">
+      <c r="F13" s="132">
         <v>1</v>
       </c>
-      <c r="G13" s="131">
+      <c r="G13" s="132">
         <v>0</v>
       </c>
-      <c r="H13" s="128">
+      <c r="H13" s="148">
         <v>1</v>
       </c>
-      <c r="I13" s="163" t="s">
+      <c r="I13" s="142" t="s">
         <v>44</v>
       </c>
-      <c r="J13" s="153"/>
-      <c r="K13" s="153"/>
-      <c r="L13" s="164"/>
-      <c r="M13" s="152" t="s">
+      <c r="J13" s="143"/>
+      <c r="K13" s="143"/>
+      <c r="L13" s="144"/>
+      <c r="M13" s="153" t="s">
         <v>129</v>
       </c>
-      <c r="N13" s="153"/>
-      <c r="O13" s="153"/>
-      <c r="P13" s="153"/>
-      <c r="Q13" s="153"/>
-      <c r="R13" s="153"/>
-      <c r="S13" s="153"/>
+      <c r="N13" s="143"/>
+      <c r="O13" s="143"/>
+      <c r="P13" s="143"/>
+      <c r="Q13" s="143"/>
+      <c r="R13" s="143"/>
+      <c r="S13" s="143"/>
       <c r="T13" s="154"/>
       <c r="V13" s="87" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="W13" s="87" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="Y13" s="87" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Z13" s="87" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="140"/>
-      <c r="B14" s="141"/>
-      <c r="C14" s="141"/>
-      <c r="D14" s="142"/>
-      <c r="E14" s="136"/>
+      <c r="A14" s="139"/>
+      <c r="B14" s="140"/>
+      <c r="C14" s="140"/>
+      <c r="D14" s="141"/>
+      <c r="E14" s="135"/>
       <c r="F14" s="133"/>
       <c r="G14" s="133"/>
-      <c r="H14" s="130"/>
-      <c r="I14" s="165"/>
-      <c r="J14" s="156"/>
-      <c r="K14" s="156"/>
-      <c r="L14" s="166"/>
+      <c r="H14" s="149"/>
+      <c r="I14" s="145"/>
+      <c r="J14" s="146"/>
+      <c r="K14" s="146"/>
+      <c r="L14" s="147"/>
       <c r="M14" s="155"/>
-      <c r="N14" s="156"/>
-      <c r="O14" s="156"/>
-      <c r="P14" s="156"/>
-      <c r="Q14" s="156"/>
-      <c r="R14" s="156"/>
-      <c r="S14" s="156"/>
-      <c r="T14" s="157"/>
+      <c r="N14" s="146"/>
+      <c r="O14" s="146"/>
+      <c r="P14" s="146"/>
+      <c r="Q14" s="146"/>
+      <c r="R14" s="146"/>
+      <c r="S14" s="146"/>
+      <c r="T14" s="156"/>
       <c r="V14" s="87" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="W14" s="87" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Y14" s="87" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Z14" s="87" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="137" t="s">
+      <c r="A15" s="136" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="138"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="139"/>
+      <c r="B15" s="137"/>
+      <c r="C15" s="137"/>
+      <c r="D15" s="138"/>
       <c r="E15" s="134">
         <v>0</v>
       </c>
-      <c r="F15" s="131">
+      <c r="F15" s="132">
         <v>1</v>
       </c>
-      <c r="G15" s="128">
+      <c r="G15" s="148">
         <v>1</v>
       </c>
-      <c r="H15" s="163" t="s">
+      <c r="H15" s="142" t="s">
         <v>123</v>
       </c>
-      <c r="I15" s="153"/>
-      <c r="J15" s="153"/>
-      <c r="K15" s="164"/>
-      <c r="L15" s="152" t="s">
+      <c r="I15" s="143"/>
+      <c r="J15" s="143"/>
+      <c r="K15" s="144"/>
+      <c r="L15" s="153" t="s">
         <v>132</v>
       </c>
-      <c r="M15" s="153"/>
-      <c r="N15" s="164"/>
-      <c r="O15" s="152" t="s">
+      <c r="M15" s="143"/>
+      <c r="N15" s="144"/>
+      <c r="O15" s="153" t="s">
         <v>133</v>
       </c>
-      <c r="P15" s="153"/>
-      <c r="Q15" s="164"/>
-      <c r="R15" s="152" t="s">
+      <c r="P15" s="143"/>
+      <c r="Q15" s="144"/>
+      <c r="R15" s="153" t="s">
         <v>134</v>
       </c>
-      <c r="S15" s="153"/>
+      <c r="S15" s="143"/>
       <c r="T15" s="154"/>
       <c r="V15" s="87" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="W15" s="87" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="Y15" s="87" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Z15" s="87" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="143"/>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="145"/>
-      <c r="E16" s="135"/>
-      <c r="F16" s="132"/>
-      <c r="G16" s="129"/>
-      <c r="H16" s="184"/>
-      <c r="I16" s="175"/>
-      <c r="J16" s="175"/>
-      <c r="K16" s="176"/>
-      <c r="L16" s="174"/>
-      <c r="M16" s="175"/>
-      <c r="N16" s="176"/>
-      <c r="O16" s="174"/>
-      <c r="P16" s="175"/>
-      <c r="Q16" s="176"/>
-      <c r="R16" s="174"/>
-      <c r="S16" s="175"/>
-      <c r="T16" s="180"/>
+      <c r="A16" s="171"/>
+      <c r="B16" s="172"/>
+      <c r="C16" s="172"/>
+      <c r="D16" s="173"/>
+      <c r="E16" s="192"/>
+      <c r="F16" s="191"/>
+      <c r="G16" s="190"/>
+      <c r="H16" s="170"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="157"/>
+      <c r="M16" s="158"/>
+      <c r="N16" s="159"/>
+      <c r="O16" s="157"/>
+      <c r="P16" s="158"/>
+      <c r="Q16" s="159"/>
+      <c r="R16" s="157"/>
+      <c r="S16" s="158"/>
+      <c r="T16" s="163"/>
       <c r="V16" s="87" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="W16" s="87" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="Y16" s="87" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Z16" s="87" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A17" s="143"/>
-      <c r="B17" s="144"/>
-      <c r="C17" s="144"/>
-      <c r="D17" s="145"/>
-      <c r="E17" s="135"/>
-      <c r="F17" s="132"/>
-      <c r="G17" s="129"/>
-      <c r="H17" s="184"/>
-      <c r="I17" s="175"/>
-      <c r="J17" s="175"/>
-      <c r="K17" s="176"/>
-      <c r="L17" s="174"/>
-      <c r="M17" s="175"/>
-      <c r="N17" s="176"/>
-      <c r="O17" s="174"/>
-      <c r="P17" s="175"/>
-      <c r="Q17" s="176"/>
-      <c r="R17" s="174"/>
-      <c r="S17" s="175"/>
-      <c r="T17" s="180"/>
+      <c r="A17" s="171"/>
+      <c r="B17" s="172"/>
+      <c r="C17" s="172"/>
+      <c r="D17" s="173"/>
+      <c r="E17" s="192"/>
+      <c r="F17" s="191"/>
+      <c r="G17" s="190"/>
+      <c r="H17" s="170"/>
+      <c r="I17" s="158"/>
+      <c r="J17" s="158"/>
+      <c r="K17" s="159"/>
+      <c r="L17" s="157"/>
+      <c r="M17" s="158"/>
+      <c r="N17" s="159"/>
+      <c r="O17" s="157"/>
+      <c r="P17" s="158"/>
+      <c r="Q17" s="159"/>
+      <c r="R17" s="157"/>
+      <c r="S17" s="158"/>
+      <c r="T17" s="163"/>
       <c r="V17" s="87" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="W17" s="87" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="Y17" s="87" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z17" s="87" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A18" s="140"/>
-      <c r="B18" s="141"/>
-      <c r="C18" s="141"/>
-      <c r="D18" s="142"/>
-      <c r="E18" s="136"/>
+      <c r="A18" s="139"/>
+      <c r="B18" s="140"/>
+      <c r="C18" s="140"/>
+      <c r="D18" s="141"/>
+      <c r="E18" s="135"/>
       <c r="F18" s="133"/>
-      <c r="G18" s="130"/>
-      <c r="H18" s="165"/>
-      <c r="I18" s="156"/>
-      <c r="J18" s="156"/>
-      <c r="K18" s="166"/>
+      <c r="G18" s="149"/>
+      <c r="H18" s="145"/>
+      <c r="I18" s="146"/>
+      <c r="J18" s="146"/>
+      <c r="K18" s="147"/>
       <c r="L18" s="155"/>
-      <c r="M18" s="156"/>
-      <c r="N18" s="166"/>
+      <c r="M18" s="146"/>
+      <c r="N18" s="147"/>
       <c r="O18" s="155"/>
-      <c r="P18" s="156"/>
-      <c r="Q18" s="166"/>
+      <c r="P18" s="146"/>
+      <c r="Q18" s="147"/>
       <c r="R18" s="155"/>
-      <c r="S18" s="156"/>
-      <c r="T18" s="157"/>
+      <c r="S18" s="146"/>
+      <c r="T18" s="156"/>
       <c r="V18" s="87" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="W18" s="87" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="Y18" s="87" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z18" s="87" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19" s="137" t="s">
+      <c r="A19" s="136" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="138"/>
-      <c r="C19" s="138"/>
-      <c r="D19" s="139"/>
-      <c r="E19" s="188">
+      <c r="B19" s="137"/>
+      <c r="C19" s="137"/>
+      <c r="D19" s="138"/>
+      <c r="E19" s="177">
         <v>1</v>
       </c>
-      <c r="F19" s="163" t="s">
+      <c r="F19" s="142" t="s">
         <v>123</v>
       </c>
-      <c r="G19" s="153"/>
-      <c r="H19" s="153"/>
-      <c r="I19" s="164"/>
-      <c r="J19" s="152" t="s">
+      <c r="G19" s="143"/>
+      <c r="H19" s="143"/>
+      <c r="I19" s="144"/>
+      <c r="J19" s="153" t="s">
         <v>132</v>
       </c>
-      <c r="K19" s="153"/>
-      <c r="L19" s="164"/>
-      <c r="M19" s="152" t="s">
+      <c r="K19" s="143"/>
+      <c r="L19" s="144"/>
+      <c r="M19" s="153" t="s">
         <v>129</v>
       </c>
-      <c r="N19" s="153"/>
-      <c r="O19" s="153"/>
-      <c r="P19" s="153"/>
-      <c r="Q19" s="153"/>
-      <c r="R19" s="153"/>
-      <c r="S19" s="153"/>
+      <c r="N19" s="143"/>
+      <c r="O19" s="143"/>
+      <c r="P19" s="143"/>
+      <c r="Q19" s="143"/>
+      <c r="R19" s="143"/>
+      <c r="S19" s="143"/>
       <c r="T19" s="154"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="143"/>
-      <c r="B20" s="144"/>
-      <c r="C20" s="144"/>
-      <c r="D20" s="145"/>
-      <c r="E20" s="189"/>
-      <c r="F20" s="184"/>
-      <c r="G20" s="175"/>
-      <c r="H20" s="175"/>
-      <c r="I20" s="176"/>
-      <c r="J20" s="174"/>
-      <c r="K20" s="175"/>
-      <c r="L20" s="176"/>
-      <c r="M20" s="174"/>
-      <c r="N20" s="175"/>
-      <c r="O20" s="175"/>
-      <c r="P20" s="175"/>
-      <c r="Q20" s="175"/>
-      <c r="R20" s="175"/>
-      <c r="S20" s="175"/>
-      <c r="T20" s="180"/>
+      <c r="A20" s="171"/>
+      <c r="B20" s="172"/>
+      <c r="C20" s="172"/>
+      <c r="D20" s="173"/>
+      <c r="E20" s="178"/>
+      <c r="F20" s="170"/>
+      <c r="G20" s="158"/>
+      <c r="H20" s="158"/>
+      <c r="I20" s="159"/>
+      <c r="J20" s="157"/>
+      <c r="K20" s="158"/>
+      <c r="L20" s="159"/>
+      <c r="M20" s="157"/>
+      <c r="N20" s="158"/>
+      <c r="O20" s="158"/>
+      <c r="P20" s="158"/>
+      <c r="Q20" s="158"/>
+      <c r="R20" s="158"/>
+      <c r="S20" s="158"/>
+      <c r="T20" s="163"/>
       <c r="V20" s="87" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21" s="143"/>
-      <c r="B21" s="144"/>
-      <c r="C21" s="144"/>
-      <c r="D21" s="145"/>
-      <c r="E21" s="189"/>
-      <c r="F21" s="184"/>
-      <c r="G21" s="175"/>
-      <c r="H21" s="175"/>
-      <c r="I21" s="176"/>
-      <c r="J21" s="174"/>
-      <c r="K21" s="175"/>
-      <c r="L21" s="176"/>
-      <c r="M21" s="174"/>
-      <c r="N21" s="175"/>
-      <c r="O21" s="175"/>
-      <c r="P21" s="175"/>
-      <c r="Q21" s="175"/>
-      <c r="R21" s="175"/>
-      <c r="S21" s="175"/>
-      <c r="T21" s="180"/>
+      <c r="A21" s="171"/>
+      <c r="B21" s="172"/>
+      <c r="C21" s="172"/>
+      <c r="D21" s="173"/>
+      <c r="E21" s="178"/>
+      <c r="F21" s="170"/>
+      <c r="G21" s="158"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="159"/>
+      <c r="J21" s="157"/>
+      <c r="K21" s="158"/>
+      <c r="L21" s="159"/>
+      <c r="M21" s="157"/>
+      <c r="N21" s="158"/>
+      <c r="O21" s="158"/>
+      <c r="P21" s="158"/>
+      <c r="Q21" s="158"/>
+      <c r="R21" s="158"/>
+      <c r="S21" s="158"/>
+      <c r="T21" s="163"/>
       <c r="V21" s="87" t="s">
         <v>58</v>
       </c>
@@ -5703,320 +5706,362 @@
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" s="143"/>
-      <c r="B22" s="144"/>
-      <c r="C22" s="144"/>
-      <c r="D22" s="145"/>
-      <c r="E22" s="189"/>
-      <c r="F22" s="184"/>
-      <c r="G22" s="175"/>
-      <c r="H22" s="175"/>
-      <c r="I22" s="176"/>
-      <c r="J22" s="174"/>
-      <c r="K22" s="175"/>
-      <c r="L22" s="176"/>
-      <c r="M22" s="174"/>
-      <c r="N22" s="175"/>
-      <c r="O22" s="175"/>
-      <c r="P22" s="175"/>
-      <c r="Q22" s="175"/>
-      <c r="R22" s="175"/>
-      <c r="S22" s="175"/>
-      <c r="T22" s="180"/>
+      <c r="A22" s="171"/>
+      <c r="B22" s="172"/>
+      <c r="C22" s="172"/>
+      <c r="D22" s="173"/>
+      <c r="E22" s="178"/>
+      <c r="F22" s="170"/>
+      <c r="G22" s="158"/>
+      <c r="H22" s="158"/>
+      <c r="I22" s="159"/>
+      <c r="J22" s="157"/>
+      <c r="K22" s="158"/>
+      <c r="L22" s="159"/>
+      <c r="M22" s="157"/>
+      <c r="N22" s="158"/>
+      <c r="O22" s="158"/>
+      <c r="P22" s="158"/>
+      <c r="Q22" s="158"/>
+      <c r="R22" s="158"/>
+      <c r="S22" s="158"/>
+      <c r="T22" s="163"/>
       <c r="V22" s="88" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="W22" s="87" t="s">
         <v>57</v>
       </c>
       <c r="X22" s="87" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A23" s="143"/>
-      <c r="B23" s="144"/>
-      <c r="C23" s="144"/>
-      <c r="D23" s="145"/>
-      <c r="E23" s="189"/>
-      <c r="F23" s="184"/>
-      <c r="G23" s="175"/>
-      <c r="H23" s="175"/>
-      <c r="I23" s="176"/>
-      <c r="J23" s="174"/>
-      <c r="K23" s="175"/>
-      <c r="L23" s="176"/>
-      <c r="M23" s="174"/>
-      <c r="N23" s="175"/>
-      <c r="O23" s="175"/>
-      <c r="P23" s="175"/>
-      <c r="Q23" s="175"/>
-      <c r="R23" s="175"/>
-      <c r="S23" s="175"/>
-      <c r="T23" s="180"/>
+      <c r="A23" s="171"/>
+      <c r="B23" s="172"/>
+      <c r="C23" s="172"/>
+      <c r="D23" s="173"/>
+      <c r="E23" s="178"/>
+      <c r="F23" s="170"/>
+      <c r="G23" s="158"/>
+      <c r="H23" s="158"/>
+      <c r="I23" s="159"/>
+      <c r="J23" s="157"/>
+      <c r="K23" s="158"/>
+      <c r="L23" s="159"/>
+      <c r="M23" s="157"/>
+      <c r="N23" s="158"/>
+      <c r="O23" s="158"/>
+      <c r="P23" s="158"/>
+      <c r="Q23" s="158"/>
+      <c r="R23" s="158"/>
+      <c r="S23" s="158"/>
+      <c r="T23" s="163"/>
       <c r="V23" s="88" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W23" s="87" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A24" s="143"/>
-      <c r="B24" s="144"/>
-      <c r="C24" s="144"/>
-      <c r="D24" s="145"/>
-      <c r="E24" s="189"/>
-      <c r="F24" s="184"/>
-      <c r="G24" s="175"/>
-      <c r="H24" s="175"/>
-      <c r="I24" s="176"/>
-      <c r="J24" s="174"/>
-      <c r="K24" s="175"/>
-      <c r="L24" s="176"/>
-      <c r="M24" s="174"/>
-      <c r="N24" s="175"/>
-      <c r="O24" s="175"/>
-      <c r="P24" s="175"/>
-      <c r="Q24" s="175"/>
-      <c r="R24" s="175"/>
-      <c r="S24" s="175"/>
-      <c r="T24" s="180"/>
+      <c r="A24" s="171"/>
+      <c r="B24" s="172"/>
+      <c r="C24" s="172"/>
+      <c r="D24" s="173"/>
+      <c r="E24" s="178"/>
+      <c r="F24" s="170"/>
+      <c r="G24" s="158"/>
+      <c r="H24" s="158"/>
+      <c r="I24" s="159"/>
+      <c r="J24" s="157"/>
+      <c r="K24" s="158"/>
+      <c r="L24" s="159"/>
+      <c r="M24" s="157"/>
+      <c r="N24" s="158"/>
+      <c r="O24" s="158"/>
+      <c r="P24" s="158"/>
+      <c r="Q24" s="158"/>
+      <c r="R24" s="158"/>
+      <c r="S24" s="158"/>
+      <c r="T24" s="163"/>
       <c r="V24" s="88" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="W24" s="87" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" s="143"/>
-      <c r="B25" s="144"/>
-      <c r="C25" s="144"/>
-      <c r="D25" s="145"/>
-      <c r="E25" s="189"/>
-      <c r="F25" s="184"/>
-      <c r="G25" s="175"/>
-      <c r="H25" s="175"/>
-      <c r="I25" s="176"/>
-      <c r="J25" s="174"/>
-      <c r="K25" s="175"/>
-      <c r="L25" s="176"/>
-      <c r="M25" s="174"/>
-      <c r="N25" s="175"/>
-      <c r="O25" s="175"/>
-      <c r="P25" s="175"/>
-      <c r="Q25" s="175"/>
-      <c r="R25" s="175"/>
-      <c r="S25" s="175"/>
-      <c r="T25" s="180"/>
+      <c r="A25" s="171"/>
+      <c r="B25" s="172"/>
+      <c r="C25" s="172"/>
+      <c r="D25" s="173"/>
+      <c r="E25" s="178"/>
+      <c r="F25" s="170"/>
+      <c r="G25" s="158"/>
+      <c r="H25" s="158"/>
+      <c r="I25" s="159"/>
+      <c r="J25" s="157"/>
+      <c r="K25" s="158"/>
+      <c r="L25" s="159"/>
+      <c r="M25" s="157"/>
+      <c r="N25" s="158"/>
+      <c r="O25" s="158"/>
+      <c r="P25" s="158"/>
+      <c r="Q25" s="158"/>
+      <c r="R25" s="158"/>
+      <c r="S25" s="158"/>
+      <c r="T25" s="163"/>
       <c r="V25" s="88" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="W25" s="87" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" s="143"/>
-      <c r="B26" s="144"/>
-      <c r="C26" s="144"/>
-      <c r="D26" s="145"/>
-      <c r="E26" s="189"/>
-      <c r="F26" s="184"/>
-      <c r="G26" s="175"/>
-      <c r="H26" s="175"/>
-      <c r="I26" s="176"/>
-      <c r="J26" s="174"/>
-      <c r="K26" s="175"/>
-      <c r="L26" s="176"/>
-      <c r="M26" s="174"/>
-      <c r="N26" s="175"/>
-      <c r="O26" s="175"/>
-      <c r="P26" s="175"/>
-      <c r="Q26" s="175"/>
-      <c r="R26" s="175"/>
-      <c r="S26" s="175"/>
-      <c r="T26" s="180"/>
+      <c r="A26" s="171"/>
+      <c r="B26" s="172"/>
+      <c r="C26" s="172"/>
+      <c r="D26" s="173"/>
+      <c r="E26" s="178"/>
+      <c r="F26" s="170"/>
+      <c r="G26" s="158"/>
+      <c r="H26" s="158"/>
+      <c r="I26" s="159"/>
+      <c r="J26" s="157"/>
+      <c r="K26" s="158"/>
+      <c r="L26" s="159"/>
+      <c r="M26" s="157"/>
+      <c r="N26" s="158"/>
+      <c r="O26" s="158"/>
+      <c r="P26" s="158"/>
+      <c r="Q26" s="158"/>
+      <c r="R26" s="158"/>
+      <c r="S26" s="158"/>
+      <c r="T26" s="163"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" s="143"/>
-      <c r="B27" s="144"/>
-      <c r="C27" s="144"/>
-      <c r="D27" s="145"/>
-      <c r="E27" s="189"/>
-      <c r="F27" s="184"/>
-      <c r="G27" s="175"/>
-      <c r="H27" s="175"/>
-      <c r="I27" s="176"/>
-      <c r="J27" s="174"/>
-      <c r="K27" s="175"/>
-      <c r="L27" s="176"/>
-      <c r="M27" s="174"/>
-      <c r="N27" s="175"/>
-      <c r="O27" s="175"/>
-      <c r="P27" s="175"/>
-      <c r="Q27" s="175"/>
-      <c r="R27" s="175"/>
-      <c r="S27" s="175"/>
-      <c r="T27" s="180"/>
+      <c r="A27" s="171"/>
+      <c r="B27" s="172"/>
+      <c r="C27" s="172"/>
+      <c r="D27" s="173"/>
+      <c r="E27" s="178"/>
+      <c r="F27" s="170"/>
+      <c r="G27" s="158"/>
+      <c r="H27" s="158"/>
+      <c r="I27" s="159"/>
+      <c r="J27" s="157"/>
+      <c r="K27" s="158"/>
+      <c r="L27" s="159"/>
+      <c r="M27" s="157"/>
+      <c r="N27" s="158"/>
+      <c r="O27" s="158"/>
+      <c r="P27" s="158"/>
+      <c r="Q27" s="158"/>
+      <c r="R27" s="158"/>
+      <c r="S27" s="158"/>
+      <c r="T27" s="163"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" s="143"/>
-      <c r="B28" s="144"/>
-      <c r="C28" s="144"/>
-      <c r="D28" s="145"/>
-      <c r="E28" s="189"/>
-      <c r="F28" s="184"/>
-      <c r="G28" s="175"/>
-      <c r="H28" s="175"/>
-      <c r="I28" s="176"/>
-      <c r="J28" s="174"/>
-      <c r="K28" s="175"/>
-      <c r="L28" s="176"/>
-      <c r="M28" s="174"/>
-      <c r="N28" s="175"/>
-      <c r="O28" s="175"/>
-      <c r="P28" s="175"/>
-      <c r="Q28" s="175"/>
-      <c r="R28" s="175"/>
-      <c r="S28" s="175"/>
-      <c r="T28" s="180"/>
+      <c r="A28" s="171"/>
+      <c r="B28" s="172"/>
+      <c r="C28" s="172"/>
+      <c r="D28" s="173"/>
+      <c r="E28" s="178"/>
+      <c r="F28" s="170"/>
+      <c r="G28" s="158"/>
+      <c r="H28" s="158"/>
+      <c r="I28" s="159"/>
+      <c r="J28" s="157"/>
+      <c r="K28" s="158"/>
+      <c r="L28" s="159"/>
+      <c r="M28" s="157"/>
+      <c r="N28" s="158"/>
+      <c r="O28" s="158"/>
+      <c r="P28" s="158"/>
+      <c r="Q28" s="158"/>
+      <c r="R28" s="158"/>
+      <c r="S28" s="158"/>
+      <c r="T28" s="163"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A29" s="143"/>
-      <c r="B29" s="144"/>
-      <c r="C29" s="144"/>
-      <c r="D29" s="145"/>
-      <c r="E29" s="189"/>
-      <c r="F29" s="184"/>
-      <c r="G29" s="175"/>
-      <c r="H29" s="175"/>
-      <c r="I29" s="176"/>
-      <c r="J29" s="174"/>
-      <c r="K29" s="175"/>
-      <c r="L29" s="176"/>
-      <c r="M29" s="174"/>
-      <c r="N29" s="175"/>
-      <c r="O29" s="175"/>
-      <c r="P29" s="175"/>
-      <c r="Q29" s="175"/>
-      <c r="R29" s="175"/>
-      <c r="S29" s="175"/>
-      <c r="T29" s="180"/>
+      <c r="A29" s="171"/>
+      <c r="B29" s="172"/>
+      <c r="C29" s="172"/>
+      <c r="D29" s="173"/>
+      <c r="E29" s="178"/>
+      <c r="F29" s="170"/>
+      <c r="G29" s="158"/>
+      <c r="H29" s="158"/>
+      <c r="I29" s="159"/>
+      <c r="J29" s="157"/>
+      <c r="K29" s="158"/>
+      <c r="L29" s="159"/>
+      <c r="M29" s="157"/>
+      <c r="N29" s="158"/>
+      <c r="O29" s="158"/>
+      <c r="P29" s="158"/>
+      <c r="Q29" s="158"/>
+      <c r="R29" s="158"/>
+      <c r="S29" s="158"/>
+      <c r="T29" s="163"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="143"/>
-      <c r="B30" s="144"/>
-      <c r="C30" s="144"/>
-      <c r="D30" s="145"/>
-      <c r="E30" s="189"/>
-      <c r="F30" s="184"/>
-      <c r="G30" s="175"/>
-      <c r="H30" s="175"/>
-      <c r="I30" s="176"/>
-      <c r="J30" s="174"/>
-      <c r="K30" s="175"/>
-      <c r="L30" s="176"/>
-      <c r="M30" s="174"/>
-      <c r="N30" s="175"/>
-      <c r="O30" s="175"/>
-      <c r="P30" s="175"/>
-      <c r="Q30" s="175"/>
-      <c r="R30" s="175"/>
-      <c r="S30" s="175"/>
-      <c r="T30" s="180"/>
+      <c r="A30" s="171"/>
+      <c r="B30" s="172"/>
+      <c r="C30" s="172"/>
+      <c r="D30" s="173"/>
+      <c r="E30" s="178"/>
+      <c r="F30" s="170"/>
+      <c r="G30" s="158"/>
+      <c r="H30" s="158"/>
+      <c r="I30" s="159"/>
+      <c r="J30" s="157"/>
+      <c r="K30" s="158"/>
+      <c r="L30" s="159"/>
+      <c r="M30" s="157"/>
+      <c r="N30" s="158"/>
+      <c r="O30" s="158"/>
+      <c r="P30" s="158"/>
+      <c r="Q30" s="158"/>
+      <c r="R30" s="158"/>
+      <c r="S30" s="158"/>
+      <c r="T30" s="163"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A31" s="143"/>
-      <c r="B31" s="144"/>
-      <c r="C31" s="144"/>
-      <c r="D31" s="145"/>
-      <c r="E31" s="189"/>
-      <c r="F31" s="184"/>
-      <c r="G31" s="175"/>
-      <c r="H31" s="175"/>
-      <c r="I31" s="176"/>
-      <c r="J31" s="174"/>
-      <c r="K31" s="175"/>
-      <c r="L31" s="176"/>
-      <c r="M31" s="174"/>
-      <c r="N31" s="175"/>
-      <c r="O31" s="175"/>
-      <c r="P31" s="175"/>
-      <c r="Q31" s="175"/>
-      <c r="R31" s="175"/>
-      <c r="S31" s="175"/>
-      <c r="T31" s="180"/>
+      <c r="A31" s="171"/>
+      <c r="B31" s="172"/>
+      <c r="C31" s="172"/>
+      <c r="D31" s="173"/>
+      <c r="E31" s="178"/>
+      <c r="F31" s="170"/>
+      <c r="G31" s="158"/>
+      <c r="H31" s="158"/>
+      <c r="I31" s="159"/>
+      <c r="J31" s="157"/>
+      <c r="K31" s="158"/>
+      <c r="L31" s="159"/>
+      <c r="M31" s="157"/>
+      <c r="N31" s="158"/>
+      <c r="O31" s="158"/>
+      <c r="P31" s="158"/>
+      <c r="Q31" s="158"/>
+      <c r="R31" s="158"/>
+      <c r="S31" s="158"/>
+      <c r="T31" s="163"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A32" s="143"/>
-      <c r="B32" s="144"/>
-      <c r="C32" s="144"/>
-      <c r="D32" s="145"/>
-      <c r="E32" s="189"/>
-      <c r="F32" s="184"/>
-      <c r="G32" s="175"/>
-      <c r="H32" s="175"/>
-      <c r="I32" s="176"/>
-      <c r="J32" s="174"/>
-      <c r="K32" s="175"/>
-      <c r="L32" s="176"/>
-      <c r="M32" s="174"/>
-      <c r="N32" s="175"/>
-      <c r="O32" s="175"/>
-      <c r="P32" s="175"/>
-      <c r="Q32" s="175"/>
-      <c r="R32" s="175"/>
-      <c r="S32" s="175"/>
-      <c r="T32" s="180"/>
+      <c r="A32" s="171"/>
+      <c r="B32" s="172"/>
+      <c r="C32" s="172"/>
+      <c r="D32" s="173"/>
+      <c r="E32" s="178"/>
+      <c r="F32" s="170"/>
+      <c r="G32" s="158"/>
+      <c r="H32" s="158"/>
+      <c r="I32" s="159"/>
+      <c r="J32" s="157"/>
+      <c r="K32" s="158"/>
+      <c r="L32" s="159"/>
+      <c r="M32" s="157"/>
+      <c r="N32" s="158"/>
+      <c r="O32" s="158"/>
+      <c r="P32" s="158"/>
+      <c r="Q32" s="158"/>
+      <c r="R32" s="158"/>
+      <c r="S32" s="158"/>
+      <c r="T32" s="163"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="143"/>
-      <c r="B33" s="144"/>
-      <c r="C33" s="144"/>
-      <c r="D33" s="145"/>
-      <c r="E33" s="189"/>
-      <c r="F33" s="184"/>
-      <c r="G33" s="175"/>
-      <c r="H33" s="175"/>
-      <c r="I33" s="176"/>
-      <c r="J33" s="174"/>
-      <c r="K33" s="175"/>
-      <c r="L33" s="176"/>
-      <c r="M33" s="174"/>
-      <c r="N33" s="175"/>
-      <c r="O33" s="175"/>
-      <c r="P33" s="175"/>
-      <c r="Q33" s="175"/>
-      <c r="R33" s="175"/>
-      <c r="S33" s="175"/>
-      <c r="T33" s="180"/>
+      <c r="A33" s="171"/>
+      <c r="B33" s="172"/>
+      <c r="C33" s="172"/>
+      <c r="D33" s="173"/>
+      <c r="E33" s="178"/>
+      <c r="F33" s="170"/>
+      <c r="G33" s="158"/>
+      <c r="H33" s="158"/>
+      <c r="I33" s="159"/>
+      <c r="J33" s="157"/>
+      <c r="K33" s="158"/>
+      <c r="L33" s="159"/>
+      <c r="M33" s="157"/>
+      <c r="N33" s="158"/>
+      <c r="O33" s="158"/>
+      <c r="P33" s="158"/>
+      <c r="Q33" s="158"/>
+      <c r="R33" s="158"/>
+      <c r="S33" s="158"/>
+      <c r="T33" s="163"/>
     </row>
     <row r="34" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="185"/>
-      <c r="B34" s="186"/>
-      <c r="C34" s="186"/>
-      <c r="D34" s="187"/>
-      <c r="E34" s="190"/>
-      <c r="F34" s="191"/>
-      <c r="G34" s="178"/>
-      <c r="H34" s="178"/>
-      <c r="I34" s="179"/>
-      <c r="J34" s="177"/>
-      <c r="K34" s="178"/>
-      <c r="L34" s="179"/>
-      <c r="M34" s="177"/>
-      <c r="N34" s="178"/>
-      <c r="O34" s="178"/>
-      <c r="P34" s="178"/>
-      <c r="Q34" s="178"/>
-      <c r="R34" s="178"/>
-      <c r="S34" s="178"/>
-      <c r="T34" s="181"/>
+      <c r="A34" s="174"/>
+      <c r="B34" s="175"/>
+      <c r="C34" s="175"/>
+      <c r="D34" s="176"/>
+      <c r="E34" s="179"/>
+      <c r="F34" s="180"/>
+      <c r="G34" s="161"/>
+      <c r="H34" s="161"/>
+      <c r="I34" s="162"/>
+      <c r="J34" s="160"/>
+      <c r="K34" s="161"/>
+      <c r="L34" s="162"/>
+      <c r="M34" s="160"/>
+      <c r="N34" s="161"/>
+      <c r="O34" s="161"/>
+      <c r="P34" s="161"/>
+      <c r="Q34" s="161"/>
+      <c r="R34" s="161"/>
+      <c r="S34" s="161"/>
+      <c r="T34" s="164"/>
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="A13:D14"/>
+    <mergeCell ref="A15:D18"/>
+    <mergeCell ref="A7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="M7:T8"/>
+    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="M5:P5"/>
+    <mergeCell ref="Q5:T5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="I7:L8"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="Q3:T3"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="M11:T12"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="J19:L34"/>
+    <mergeCell ref="M19:T34"/>
+    <mergeCell ref="K9:T9"/>
+    <mergeCell ref="J10:T10"/>
+    <mergeCell ref="M13:T14"/>
+    <mergeCell ref="I13:L14"/>
+    <mergeCell ref="L15:N18"/>
+    <mergeCell ref="O15:Q18"/>
+    <mergeCell ref="R15:T18"/>
+    <mergeCell ref="H15:K18"/>
+    <mergeCell ref="A19:D34"/>
+    <mergeCell ref="E19:E34"/>
+    <mergeCell ref="F19:I34"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="C6:D6"/>
@@ -6033,48 +6078,6 @@
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="H11:H12"/>
-    <mergeCell ref="M11:T12"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="J19:L34"/>
-    <mergeCell ref="M19:T34"/>
-    <mergeCell ref="K9:T9"/>
-    <mergeCell ref="J10:T10"/>
-    <mergeCell ref="M13:T14"/>
-    <mergeCell ref="I13:L14"/>
-    <mergeCell ref="L15:N18"/>
-    <mergeCell ref="O15:Q18"/>
-    <mergeCell ref="R15:T18"/>
-    <mergeCell ref="H15:K18"/>
-    <mergeCell ref="A19:D34"/>
-    <mergeCell ref="E19:E34"/>
-    <mergeCell ref="F19:I34"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="Q3:T3"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="M7:T8"/>
-    <mergeCell ref="O6:T6"/>
-    <mergeCell ref="M5:P5"/>
-    <mergeCell ref="Q5:T5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="I7:L8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="A13:D14"/>
-    <mergeCell ref="A15:D18"/>
-    <mergeCell ref="A7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6141,26 +6144,26 @@
         <v>41</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C3" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="D3" s="35" t="s">
         <v>248</v>
-      </c>
-      <c r="D3" s="35" t="s">
-        <v>249</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="G3" s="37"/>
       <c r="J3" s="88" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K3" s="87" t="s">
         <v>57</v>
       </c>
       <c r="L3" s="87" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N3" s="17"/>
     </row>
@@ -6169,20 +6172,20 @@
         <v>42</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C4" s="37" t="s">
+        <v>247</v>
+      </c>
+      <c r="D4" s="38" t="s">
         <v>248</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>249</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="G4" s="37"/>
       <c r="J4" s="88" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K4" s="87" t="s">
         <v>55</v>
@@ -6198,14 +6201,14 @@
         <v>44</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D5" s="25"/>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="J5" s="88" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K5" s="87" t="s">
         <v>54</v>
@@ -6221,14 +6224,14 @@
         <v>44</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="J6" s="88" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K6" s="87" t="s">
         <v>56</v>
@@ -6241,7 +6244,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C7" s="31" t="s">
         <v>47</v>
@@ -6254,10 +6257,10 @@
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C8" s="89"/>
       <c r="D8" s="5"/>
@@ -6286,10 +6289,10 @@
         <v>48</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D10" s="28"/>
       <c r="E10">
@@ -6305,10 +6308,10 @@
         <v>44</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -6323,7 +6326,7 @@
         <v>44</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12">
@@ -6339,10 +6342,10 @@
         <v>44</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -6358,10 +6361,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="C14" s="27" t="s">
         <v>251</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>252</v>
       </c>
       <c r="D14" s="90"/>
       <c r="E14">
@@ -6374,10 +6377,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="C15" s="37" t="s">
         <v>251</v>
-      </c>
-      <c r="C15" s="37" t="s">
-        <v>252</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15">
@@ -6390,10 +6393,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="C16" s="37" t="s">
         <v>251</v>
-      </c>
-      <c r="C16" s="37" t="s">
-        <v>252</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16">
@@ -6406,10 +6409,10 @@
         <v>31</v>
       </c>
       <c r="B17" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="C17" s="37" t="s">
         <v>251</v>
-      </c>
-      <c r="C17" s="37" t="s">
-        <v>252</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17">
@@ -6422,10 +6425,10 @@
         <v>33</v>
       </c>
       <c r="B18" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="C18" s="37" t="s">
         <v>251</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>252</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18">
@@ -6437,10 +6440,10 @@
         <v>34</v>
       </c>
       <c r="B19" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="C19" s="37" t="s">
         <v>251</v>
-      </c>
-      <c r="C19" s="37" t="s">
-        <v>252</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19">
@@ -6449,13 +6452,13 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B20" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="C20" s="37" t="s">
         <v>251</v>
-      </c>
-      <c r="C20" s="37" t="s">
-        <v>252</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20">
@@ -6464,13 +6467,13 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B21" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="C21" s="37" t="s">
         <v>251</v>
-      </c>
-      <c r="C21" s="37" t="s">
-        <v>252</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21">
@@ -6482,10 +6485,10 @@
         <v>16</v>
       </c>
       <c r="B22" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="C22" s="37" t="s">
         <v>251</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>252</v>
       </c>
       <c r="D22" s="25"/>
       <c r="E22">
@@ -6497,10 +6500,10 @@
         <v>19</v>
       </c>
       <c r="B23" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="C23" s="37" t="s">
         <v>251</v>
-      </c>
-      <c r="C23" s="37" t="s">
-        <v>252</v>
       </c>
       <c r="D23" s="25"/>
       <c r="E23">
@@ -6512,10 +6515,10 @@
         <v>21</v>
       </c>
       <c r="B24" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="C24" s="37" t="s">
         <v>251</v>
-      </c>
-      <c r="C24" s="37" t="s">
-        <v>252</v>
       </c>
       <c r="D24" s="25"/>
       <c r="E24">
@@ -6524,13 +6527,13 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B25" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="C25" s="37" t="s">
         <v>251</v>
-      </c>
-      <c r="C25" s="37" t="s">
-        <v>252</v>
       </c>
       <c r="D25" s="25"/>
       <c r="E25">
@@ -6542,10 +6545,10 @@
         <v>23</v>
       </c>
       <c r="B26" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="C26" s="37" t="s">
         <v>251</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>252</v>
       </c>
       <c r="D26" s="25"/>
       <c r="E26">
@@ -6557,10 +6560,10 @@
         <v>29</v>
       </c>
       <c r="B27" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="C27" s="37" t="s">
         <v>251</v>
-      </c>
-      <c r="C27" s="37" t="s">
-        <v>252</v>
       </c>
       <c r="D27" s="25"/>
       <c r="E27">
@@ -6572,10 +6575,10 @@
         <v>26</v>
       </c>
       <c r="B28" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="C28" s="37" t="s">
         <v>251</v>
-      </c>
-      <c r="C28" s="37" t="s">
-        <v>252</v>
       </c>
       <c r="D28" s="25"/>
       <c r="E28">
@@ -6587,10 +6590,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="C29" s="30" t="s">
         <v>251</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>252</v>
       </c>
       <c r="D29" s="32"/>
       <c r="E29">
@@ -6752,7 +6755,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>33</v>
@@ -6775,7 +6778,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>34</v>
@@ -6798,10 +6801,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>9</v>
@@ -6821,10 +6824,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>17</v>
@@ -6916,7 +6919,7 @@
         <v>32</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Internal Bus Complex is completed
</commit_message>
<xml_diff>
--- a/Instruction Set/InstSet.xlsx
+++ b/Instruction Set/InstSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cemal\Documents\GitHub\myCPU\Instruction Set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7819E4ED-1156-4FD7-903B-EFB23B7C0F47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D762DE13-89B1-40F8-969C-CB9D4993DB33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="301">
   <si>
     <t>S3</t>
   </si>
@@ -2264,192 +2264,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="57" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="29" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="58" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="27" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="30" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="44" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="46" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="40" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="33" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="38" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="37" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2459,13 +2273,67 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="57" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="29" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="58" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="27" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="40" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="33" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="46" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2476,6 +2344,138 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="30" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="44" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="38" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="37" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2777,8 +2777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0587EB1-1C15-4BDC-B095-DE818FDD326C}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3715,7 +3715,7 @@
   <dimension ref="A1:U45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4384,7 +4384,7 @@
         <v>161</v>
       </c>
       <c r="N20" s="46" t="s">
-        <v>213</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -4416,7 +4416,7 @@
         <v>162</v>
       </c>
       <c r="N21" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -4452,7 +4452,7 @@
         <v>166</v>
       </c>
       <c r="N22" s="46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -4483,6 +4483,12 @@
       </c>
       <c r="J23" s="83" t="s">
         <v>161</v>
+      </c>
+      <c r="M23" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="N23" s="46" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -4623,7 +4629,7 @@
         <v>57</v>
       </c>
       <c r="E32" s="83" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -4638,7 +4644,7 @@
         <v>54</v>
       </c>
       <c r="E33" s="83" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -4653,7 +4659,7 @@
         <v>56</v>
       </c>
       <c r="E34" s="83" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -4670,7 +4676,7 @@
         <v>56</v>
       </c>
       <c r="E35" s="83" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4685,7 +4691,7 @@
         <v>56</v>
       </c>
       <c r="E36" s="76" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4790,12 +4796,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="187" t="s">
+      <c r="A1" s="125" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="188"/>
-      <c r="C1" s="188"/>
-      <c r="D1" s="189"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="127"/>
       <c r="E1" s="91">
         <v>15</v>
       </c>
@@ -4873,23 +4879,23 @@
       <c r="I2" s="100">
         <v>0</v>
       </c>
-      <c r="J2" s="125" t="s">
+      <c r="J2" s="192" t="s">
         <v>123</v>
       </c>
-      <c r="K2" s="126"/>
-      <c r="L2" s="127"/>
-      <c r="M2" s="181" t="s">
+      <c r="K2" s="193"/>
+      <c r="L2" s="194"/>
+      <c r="M2" s="167" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="182"/>
-      <c r="O2" s="182"/>
-      <c r="P2" s="182"/>
-      <c r="Q2" s="182" t="s">
+      <c r="N2" s="168"/>
+      <c r="O2" s="168"/>
+      <c r="P2" s="168"/>
+      <c r="Q2" s="168" t="s">
         <v>124</v>
       </c>
-      <c r="R2" s="182"/>
-      <c r="S2" s="182"/>
-      <c r="T2" s="183"/>
+      <c r="R2" s="168"/>
+      <c r="S2" s="168"/>
+      <c r="T2" s="169"/>
       <c r="V2" s="87" t="s">
         <v>81</v>
       </c>
@@ -4925,23 +4931,23 @@
       <c r="I3" s="105">
         <v>1</v>
       </c>
-      <c r="J3" s="128" t="s">
+      <c r="J3" s="170" t="s">
         <v>123</v>
       </c>
-      <c r="K3" s="128"/>
-      <c r="L3" s="129"/>
-      <c r="M3" s="184" t="s">
+      <c r="K3" s="170"/>
+      <c r="L3" s="195"/>
+      <c r="M3" s="161" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="128"/>
-      <c r="O3" s="128"/>
-      <c r="P3" s="128"/>
-      <c r="Q3" s="128" t="s">
+      <c r="N3" s="170"/>
+      <c r="O3" s="170"/>
+      <c r="P3" s="170"/>
+      <c r="Q3" s="170" t="s">
         <v>124</v>
       </c>
-      <c r="R3" s="128"/>
-      <c r="S3" s="128"/>
-      <c r="T3" s="185"/>
+      <c r="R3" s="170"/>
+      <c r="S3" s="170"/>
+      <c r="T3" s="171"/>
       <c r="V3" s="87" t="s">
         <v>267</v>
       </c>
@@ -4959,11 +4965,11 @@
       <c r="A4" s="107" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="130" t="s">
+      <c r="B4" s="146" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="152"/>
-      <c r="D4" s="131"/>
+      <c r="C4" s="147"/>
+      <c r="D4" s="148"/>
       <c r="E4" s="104">
         <v>0</v>
       </c>
@@ -4982,22 +4988,22 @@
       <c r="J4" s="120">
         <v>0</v>
       </c>
-      <c r="K4" s="128" t="s">
+      <c r="K4" s="170" t="s">
         <v>123</v>
       </c>
-      <c r="L4" s="129"/>
-      <c r="M4" s="184" t="s">
+      <c r="L4" s="195"/>
+      <c r="M4" s="161" t="s">
         <v>122</v>
       </c>
-      <c r="N4" s="128"/>
-      <c r="O4" s="128"/>
-      <c r="P4" s="128"/>
-      <c r="Q4" s="128" t="s">
+      <c r="N4" s="170"/>
+      <c r="O4" s="170"/>
+      <c r="P4" s="170"/>
+      <c r="Q4" s="170" t="s">
         <v>44</v>
       </c>
-      <c r="R4" s="128"/>
-      <c r="S4" s="128"/>
-      <c r="T4" s="185"/>
+      <c r="R4" s="170"/>
+      <c r="S4" s="170"/>
+      <c r="T4" s="171"/>
       <c r="V4" s="87" t="s">
         <v>268</v>
       </c>
@@ -5012,12 +5018,12 @@
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="193" t="s">
+      <c r="A5" s="149" t="s">
         <v>242</v>
       </c>
-      <c r="B5" s="194"/>
-      <c r="C5" s="194"/>
-      <c r="D5" s="195"/>
+      <c r="B5" s="150"/>
+      <c r="C5" s="150"/>
+      <c r="D5" s="151"/>
       <c r="E5" s="104">
         <v>0</v>
       </c>
@@ -5036,22 +5042,22 @@
       <c r="J5" s="124">
         <v>1</v>
       </c>
-      <c r="K5" s="165" t="s">
+      <c r="K5" s="162" t="s">
         <v>171</v>
       </c>
-      <c r="L5" s="184"/>
-      <c r="M5" s="186" t="s">
+      <c r="L5" s="161"/>
+      <c r="M5" s="158" t="s">
         <v>124</v>
       </c>
-      <c r="N5" s="166"/>
-      <c r="O5" s="166"/>
-      <c r="P5" s="184"/>
-      <c r="Q5" s="186" t="s">
+      <c r="N5" s="159"/>
+      <c r="O5" s="159"/>
+      <c r="P5" s="161"/>
+      <c r="Q5" s="158" t="s">
         <v>172</v>
       </c>
-      <c r="R5" s="166"/>
-      <c r="S5" s="166"/>
-      <c r="T5" s="167"/>
+      <c r="R5" s="159"/>
+      <c r="S5" s="159"/>
+      <c r="T5" s="160"/>
       <c r="V5" s="87" t="s">
         <v>269</v>
       </c>
@@ -5066,14 +5072,14 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="150" t="s">
+      <c r="A6" s="172" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="151"/>
-      <c r="C6" s="130" t="s">
+      <c r="B6" s="173"/>
+      <c r="C6" s="146" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="131"/>
+      <c r="D6" s="148"/>
       <c r="E6" s="104">
         <v>0</v>
       </c>
@@ -5092,20 +5098,20 @@
       <c r="J6" s="124" t="s">
         <v>123</v>
       </c>
-      <c r="K6" s="165" t="s">
+      <c r="K6" s="162" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="166"/>
-      <c r="M6" s="166"/>
-      <c r="N6" s="184"/>
-      <c r="O6" s="186" t="s">
+      <c r="L6" s="159"/>
+      <c r="M6" s="159"/>
+      <c r="N6" s="161"/>
+      <c r="O6" s="158" t="s">
         <v>130</v>
       </c>
-      <c r="P6" s="166"/>
-      <c r="Q6" s="166"/>
-      <c r="R6" s="166"/>
-      <c r="S6" s="166"/>
-      <c r="T6" s="167"/>
+      <c r="P6" s="159"/>
+      <c r="Q6" s="159"/>
+      <c r="R6" s="159"/>
+      <c r="S6" s="159"/>
+      <c r="T6" s="160"/>
       <c r="V6" s="87" t="s">
         <v>270</v>
       </c>
@@ -5120,39 +5126,39 @@
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="136" t="s">
+      <c r="A7" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="137"/>
-      <c r="C7" s="137"/>
-      <c r="D7" s="138"/>
+      <c r="B7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="139"/>
       <c r="E7" s="134">
         <v>0</v>
       </c>
-      <c r="F7" s="132">
+      <c r="F7" s="131">
         <v>0</v>
       </c>
-      <c r="G7" s="132">
+      <c r="G7" s="131">
         <v>1</v>
       </c>
-      <c r="H7" s="148">
+      <c r="H7" s="128">
         <v>0</v>
       </c>
-      <c r="I7" s="142" t="s">
+      <c r="I7" s="163" t="s">
         <v>122</v>
       </c>
-      <c r="J7" s="143"/>
-      <c r="K7" s="143"/>
-      <c r="L7" s="144"/>
-      <c r="M7" s="153" t="s">
+      <c r="J7" s="153"/>
+      <c r="K7" s="153"/>
+      <c r="L7" s="164"/>
+      <c r="M7" s="152" t="s">
         <v>129</v>
       </c>
-      <c r="N7" s="143"/>
-      <c r="O7" s="143"/>
-      <c r="P7" s="143"/>
-      <c r="Q7" s="143"/>
-      <c r="R7" s="143"/>
-      <c r="S7" s="143"/>
+      <c r="N7" s="153"/>
+      <c r="O7" s="153"/>
+      <c r="P7" s="153"/>
+      <c r="Q7" s="153"/>
+      <c r="R7" s="153"/>
+      <c r="S7" s="153"/>
       <c r="T7" s="154"/>
       <c r="V7" s="87" t="s">
         <v>271</v>
@@ -5168,26 +5174,26 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="139"/>
-      <c r="B8" s="140"/>
-      <c r="C8" s="140"/>
-      <c r="D8" s="141"/>
-      <c r="E8" s="135"/>
+      <c r="A8" s="140"/>
+      <c r="B8" s="141"/>
+      <c r="C8" s="141"/>
+      <c r="D8" s="142"/>
+      <c r="E8" s="136"/>
       <c r="F8" s="133"/>
       <c r="G8" s="133"/>
-      <c r="H8" s="149"/>
-      <c r="I8" s="145"/>
-      <c r="J8" s="146"/>
-      <c r="K8" s="146"/>
-      <c r="L8" s="147"/>
+      <c r="H8" s="130"/>
+      <c r="I8" s="165"/>
+      <c r="J8" s="156"/>
+      <c r="K8" s="156"/>
+      <c r="L8" s="166"/>
       <c r="M8" s="155"/>
-      <c r="N8" s="146"/>
-      <c r="O8" s="146"/>
-      <c r="P8" s="146"/>
-      <c r="Q8" s="146"/>
-      <c r="R8" s="146"/>
-      <c r="S8" s="146"/>
-      <c r="T8" s="156"/>
+      <c r="N8" s="156"/>
+      <c r="O8" s="156"/>
+      <c r="P8" s="156"/>
+      <c r="Q8" s="156"/>
+      <c r="R8" s="156"/>
+      <c r="S8" s="156"/>
+      <c r="T8" s="157"/>
       <c r="V8" s="87" t="s">
         <v>272</v>
       </c>
@@ -5202,14 +5208,14 @@
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="150" t="s">
+      <c r="A9" s="172" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="151"/>
-      <c r="C9" s="130" t="s">
+      <c r="B9" s="173"/>
+      <c r="C9" s="146" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="131"/>
+      <c r="D9" s="148"/>
       <c r="E9" s="104">
         <v>0</v>
       </c>
@@ -5228,18 +5234,18 @@
       <c r="J9" s="124" t="s">
         <v>123</v>
       </c>
-      <c r="K9" s="165" t="s">
+      <c r="K9" s="162" t="s">
         <v>131</v>
       </c>
-      <c r="L9" s="166"/>
-      <c r="M9" s="166"/>
-      <c r="N9" s="166"/>
-      <c r="O9" s="166"/>
-      <c r="P9" s="166"/>
-      <c r="Q9" s="166"/>
-      <c r="R9" s="166"/>
-      <c r="S9" s="166"/>
-      <c r="T9" s="167"/>
+      <c r="L9" s="159"/>
+      <c r="M9" s="159"/>
+      <c r="N9" s="159"/>
+      <c r="O9" s="159"/>
+      <c r="P9" s="159"/>
+      <c r="Q9" s="159"/>
+      <c r="R9" s="159"/>
+      <c r="S9" s="159"/>
+      <c r="T9" s="160"/>
       <c r="V9" s="87" t="s">
         <v>273</v>
       </c>
@@ -5254,12 +5260,12 @@
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="150" t="s">
+      <c r="A10" s="172" t="s">
         <v>230</v>
       </c>
-      <c r="B10" s="152"/>
-      <c r="C10" s="152"/>
-      <c r="D10" s="131"/>
+      <c r="B10" s="147"/>
+      <c r="C10" s="147"/>
+      <c r="D10" s="148"/>
       <c r="E10" s="104">
         <v>0</v>
       </c>
@@ -5275,19 +5281,19 @@
       <c r="I10" s="106">
         <v>1</v>
       </c>
-      <c r="J10" s="168" t="s">
+      <c r="J10" s="182" t="s">
         <v>137</v>
       </c>
-      <c r="K10" s="168"/>
-      <c r="L10" s="168"/>
-      <c r="M10" s="168"/>
-      <c r="N10" s="168"/>
-      <c r="O10" s="168"/>
-      <c r="P10" s="168"/>
-      <c r="Q10" s="168"/>
-      <c r="R10" s="168"/>
-      <c r="S10" s="168"/>
-      <c r="T10" s="169"/>
+      <c r="K10" s="182"/>
+      <c r="L10" s="182"/>
+      <c r="M10" s="182"/>
+      <c r="N10" s="182"/>
+      <c r="O10" s="182"/>
+      <c r="P10" s="182"/>
+      <c r="Q10" s="182"/>
+      <c r="R10" s="182"/>
+      <c r="S10" s="182"/>
+      <c r="T10" s="183"/>
       <c r="V10" s="87" t="s">
         <v>274</v>
       </c>
@@ -5302,39 +5308,39 @@
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="136" t="s">
+      <c r="A11" s="137" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="137"/>
-      <c r="C11" s="137"/>
-      <c r="D11" s="138"/>
+      <c r="B11" s="138"/>
+      <c r="C11" s="138"/>
+      <c r="D11" s="139"/>
       <c r="E11" s="134">
         <v>0</v>
       </c>
-      <c r="F11" s="132">
+      <c r="F11" s="131">
         <v>1</v>
       </c>
-      <c r="G11" s="132">
+      <c r="G11" s="131">
         <v>0</v>
       </c>
-      <c r="H11" s="148">
+      <c r="H11" s="128">
         <v>0</v>
       </c>
-      <c r="I11" s="142" t="s">
+      <c r="I11" s="163" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="143"/>
-      <c r="K11" s="143"/>
-      <c r="L11" s="144"/>
-      <c r="M11" s="153" t="s">
+      <c r="J11" s="153"/>
+      <c r="K11" s="153"/>
+      <c r="L11" s="164"/>
+      <c r="M11" s="152" t="s">
         <v>129</v>
       </c>
-      <c r="N11" s="143"/>
-      <c r="O11" s="143"/>
-      <c r="P11" s="143"/>
-      <c r="Q11" s="143"/>
-      <c r="R11" s="143"/>
-      <c r="S11" s="143"/>
+      <c r="N11" s="153"/>
+      <c r="O11" s="153"/>
+      <c r="P11" s="153"/>
+      <c r="Q11" s="153"/>
+      <c r="R11" s="153"/>
+      <c r="S11" s="153"/>
       <c r="T11" s="154"/>
       <c r="V11" s="87" t="s">
         <v>275</v>
@@ -5350,26 +5356,26 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="139"/>
-      <c r="B12" s="140"/>
-      <c r="C12" s="140"/>
-      <c r="D12" s="141"/>
-      <c r="E12" s="135"/>
+      <c r="A12" s="140"/>
+      <c r="B12" s="141"/>
+      <c r="C12" s="141"/>
+      <c r="D12" s="142"/>
+      <c r="E12" s="136"/>
       <c r="F12" s="133"/>
       <c r="G12" s="133"/>
-      <c r="H12" s="149"/>
-      <c r="I12" s="145"/>
-      <c r="J12" s="146"/>
-      <c r="K12" s="146"/>
-      <c r="L12" s="147"/>
+      <c r="H12" s="130"/>
+      <c r="I12" s="165"/>
+      <c r="J12" s="156"/>
+      <c r="K12" s="156"/>
+      <c r="L12" s="166"/>
       <c r="M12" s="155"/>
-      <c r="N12" s="146"/>
-      <c r="O12" s="146"/>
-      <c r="P12" s="146"/>
-      <c r="Q12" s="146"/>
-      <c r="R12" s="146"/>
-      <c r="S12" s="146"/>
-      <c r="T12" s="156"/>
+      <c r="N12" s="156"/>
+      <c r="O12" s="156"/>
+      <c r="P12" s="156"/>
+      <c r="Q12" s="156"/>
+      <c r="R12" s="156"/>
+      <c r="S12" s="156"/>
+      <c r="T12" s="157"/>
       <c r="V12" s="87" t="s">
         <v>276</v>
       </c>
@@ -5384,39 +5390,39 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="136" t="s">
+      <c r="A13" s="137" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="137"/>
-      <c r="C13" s="137"/>
-      <c r="D13" s="138"/>
+      <c r="B13" s="138"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="139"/>
       <c r="E13" s="134">
         <v>0</v>
       </c>
-      <c r="F13" s="132">
+      <c r="F13" s="131">
         <v>1</v>
       </c>
-      <c r="G13" s="132">
+      <c r="G13" s="131">
         <v>0</v>
       </c>
-      <c r="H13" s="148">
+      <c r="H13" s="128">
         <v>1</v>
       </c>
-      <c r="I13" s="142" t="s">
+      <c r="I13" s="163" t="s">
         <v>44</v>
       </c>
-      <c r="J13" s="143"/>
-      <c r="K13" s="143"/>
-      <c r="L13" s="144"/>
-      <c r="M13" s="153" t="s">
+      <c r="J13" s="153"/>
+      <c r="K13" s="153"/>
+      <c r="L13" s="164"/>
+      <c r="M13" s="152" t="s">
         <v>129</v>
       </c>
-      <c r="N13" s="143"/>
-      <c r="O13" s="143"/>
-      <c r="P13" s="143"/>
-      <c r="Q13" s="143"/>
-      <c r="R13" s="143"/>
-      <c r="S13" s="143"/>
+      <c r="N13" s="153"/>
+      <c r="O13" s="153"/>
+      <c r="P13" s="153"/>
+      <c r="Q13" s="153"/>
+      <c r="R13" s="153"/>
+      <c r="S13" s="153"/>
       <c r="T13" s="154"/>
       <c r="V13" s="87" t="s">
         <v>277</v>
@@ -5432,26 +5438,26 @@
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="139"/>
-      <c r="B14" s="140"/>
-      <c r="C14" s="140"/>
-      <c r="D14" s="141"/>
-      <c r="E14" s="135"/>
+      <c r="A14" s="140"/>
+      <c r="B14" s="141"/>
+      <c r="C14" s="141"/>
+      <c r="D14" s="142"/>
+      <c r="E14" s="136"/>
       <c r="F14" s="133"/>
       <c r="G14" s="133"/>
-      <c r="H14" s="149"/>
-      <c r="I14" s="145"/>
-      <c r="J14" s="146"/>
-      <c r="K14" s="146"/>
-      <c r="L14" s="147"/>
+      <c r="H14" s="130"/>
+      <c r="I14" s="165"/>
+      <c r="J14" s="156"/>
+      <c r="K14" s="156"/>
+      <c r="L14" s="166"/>
       <c r="M14" s="155"/>
-      <c r="N14" s="146"/>
-      <c r="O14" s="146"/>
-      <c r="P14" s="146"/>
-      <c r="Q14" s="146"/>
-      <c r="R14" s="146"/>
-      <c r="S14" s="146"/>
-      <c r="T14" s="156"/>
+      <c r="N14" s="156"/>
+      <c r="O14" s="156"/>
+      <c r="P14" s="156"/>
+      <c r="Q14" s="156"/>
+      <c r="R14" s="156"/>
+      <c r="S14" s="156"/>
+      <c r="T14" s="157"/>
       <c r="V14" s="87" t="s">
         <v>278</v>
       </c>
@@ -5466,41 +5472,41 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="136" t="s">
+      <c r="A15" s="137" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="137"/>
-      <c r="C15" s="137"/>
-      <c r="D15" s="138"/>
+      <c r="B15" s="138"/>
+      <c r="C15" s="138"/>
+      <c r="D15" s="139"/>
       <c r="E15" s="134">
         <v>0</v>
       </c>
-      <c r="F15" s="132">
+      <c r="F15" s="131">
         <v>1</v>
       </c>
-      <c r="G15" s="148">
+      <c r="G15" s="128">
         <v>1</v>
       </c>
-      <c r="H15" s="142" t="s">
+      <c r="H15" s="163" t="s">
         <v>123</v>
       </c>
-      <c r="I15" s="143"/>
-      <c r="J15" s="143"/>
-      <c r="K15" s="144"/>
-      <c r="L15" s="153" t="s">
+      <c r="I15" s="153"/>
+      <c r="J15" s="153"/>
+      <c r="K15" s="164"/>
+      <c r="L15" s="152" t="s">
         <v>132</v>
       </c>
-      <c r="M15" s="143"/>
-      <c r="N15" s="144"/>
-      <c r="O15" s="153" t="s">
+      <c r="M15" s="153"/>
+      <c r="N15" s="164"/>
+      <c r="O15" s="152" t="s">
         <v>133</v>
       </c>
-      <c r="P15" s="143"/>
-      <c r="Q15" s="144"/>
-      <c r="R15" s="153" t="s">
+      <c r="P15" s="153"/>
+      <c r="Q15" s="164"/>
+      <c r="R15" s="152" t="s">
         <v>134</v>
       </c>
-      <c r="S15" s="143"/>
+      <c r="S15" s="153"/>
       <c r="T15" s="154"/>
       <c r="V15" s="87" t="s">
         <v>279</v>
@@ -5516,26 +5522,26 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="171"/>
-      <c r="B16" s="172"/>
-      <c r="C16" s="172"/>
-      <c r="D16" s="173"/>
-      <c r="E16" s="192"/>
-      <c r="F16" s="191"/>
-      <c r="G16" s="190"/>
-      <c r="H16" s="170"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="157"/>
-      <c r="M16" s="158"/>
-      <c r="N16" s="159"/>
-      <c r="O16" s="157"/>
-      <c r="P16" s="158"/>
-      <c r="Q16" s="159"/>
-      <c r="R16" s="157"/>
-      <c r="S16" s="158"/>
-      <c r="T16" s="163"/>
+      <c r="A16" s="143"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="145"/>
+      <c r="E16" s="135"/>
+      <c r="F16" s="132"/>
+      <c r="G16" s="129"/>
+      <c r="H16" s="184"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="176"/>
+      <c r="L16" s="174"/>
+      <c r="M16" s="175"/>
+      <c r="N16" s="176"/>
+      <c r="O16" s="174"/>
+      <c r="P16" s="175"/>
+      <c r="Q16" s="176"/>
+      <c r="R16" s="174"/>
+      <c r="S16" s="175"/>
+      <c r="T16" s="180"/>
       <c r="V16" s="87" t="s">
         <v>280</v>
       </c>
@@ -5550,26 +5556,26 @@
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A17" s="171"/>
-      <c r="B17" s="172"/>
-      <c r="C17" s="172"/>
-      <c r="D17" s="173"/>
-      <c r="E17" s="192"/>
-      <c r="F17" s="191"/>
-      <c r="G17" s="190"/>
-      <c r="H17" s="170"/>
-      <c r="I17" s="158"/>
-      <c r="J17" s="158"/>
-      <c r="K17" s="159"/>
-      <c r="L17" s="157"/>
-      <c r="M17" s="158"/>
-      <c r="N17" s="159"/>
-      <c r="O17" s="157"/>
-      <c r="P17" s="158"/>
-      <c r="Q17" s="159"/>
-      <c r="R17" s="157"/>
-      <c r="S17" s="158"/>
-      <c r="T17" s="163"/>
+      <c r="A17" s="143"/>
+      <c r="B17" s="144"/>
+      <c r="C17" s="144"/>
+      <c r="D17" s="145"/>
+      <c r="E17" s="135"/>
+      <c r="F17" s="132"/>
+      <c r="G17" s="129"/>
+      <c r="H17" s="184"/>
+      <c r="I17" s="175"/>
+      <c r="J17" s="175"/>
+      <c r="K17" s="176"/>
+      <c r="L17" s="174"/>
+      <c r="M17" s="175"/>
+      <c r="N17" s="176"/>
+      <c r="O17" s="174"/>
+      <c r="P17" s="175"/>
+      <c r="Q17" s="176"/>
+      <c r="R17" s="174"/>
+      <c r="S17" s="175"/>
+      <c r="T17" s="180"/>
       <c r="V17" s="87" t="s">
         <v>281</v>
       </c>
@@ -5584,26 +5590,26 @@
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A18" s="139"/>
-      <c r="B18" s="140"/>
-      <c r="C18" s="140"/>
-      <c r="D18" s="141"/>
-      <c r="E18" s="135"/>
+      <c r="A18" s="140"/>
+      <c r="B18" s="141"/>
+      <c r="C18" s="141"/>
+      <c r="D18" s="142"/>
+      <c r="E18" s="136"/>
       <c r="F18" s="133"/>
-      <c r="G18" s="149"/>
-      <c r="H18" s="145"/>
-      <c r="I18" s="146"/>
-      <c r="J18" s="146"/>
-      <c r="K18" s="147"/>
+      <c r="G18" s="130"/>
+      <c r="H18" s="165"/>
+      <c r="I18" s="156"/>
+      <c r="J18" s="156"/>
+      <c r="K18" s="166"/>
       <c r="L18" s="155"/>
-      <c r="M18" s="146"/>
-      <c r="N18" s="147"/>
+      <c r="M18" s="156"/>
+      <c r="N18" s="166"/>
       <c r="O18" s="155"/>
-      <c r="P18" s="146"/>
-      <c r="Q18" s="147"/>
+      <c r="P18" s="156"/>
+      <c r="Q18" s="166"/>
       <c r="R18" s="155"/>
-      <c r="S18" s="146"/>
-      <c r="T18" s="156"/>
+      <c r="S18" s="156"/>
+      <c r="T18" s="157"/>
       <c r="V18" s="87" t="s">
         <v>282</v>
       </c>
@@ -5618,83 +5624,83 @@
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19" s="136" t="s">
+      <c r="A19" s="137" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="137"/>
-      <c r="C19" s="137"/>
-      <c r="D19" s="138"/>
-      <c r="E19" s="177">
+      <c r="B19" s="138"/>
+      <c r="C19" s="138"/>
+      <c r="D19" s="139"/>
+      <c r="E19" s="188">
         <v>1</v>
       </c>
-      <c r="F19" s="142" t="s">
+      <c r="F19" s="163" t="s">
         <v>123</v>
       </c>
-      <c r="G19" s="143"/>
-      <c r="H19" s="143"/>
-      <c r="I19" s="144"/>
-      <c r="J19" s="153" t="s">
+      <c r="G19" s="153"/>
+      <c r="H19" s="153"/>
+      <c r="I19" s="164"/>
+      <c r="J19" s="152" t="s">
         <v>132</v>
       </c>
-      <c r="K19" s="143"/>
-      <c r="L19" s="144"/>
-      <c r="M19" s="153" t="s">
+      <c r="K19" s="153"/>
+      <c r="L19" s="164"/>
+      <c r="M19" s="152" t="s">
         <v>129</v>
       </c>
-      <c r="N19" s="143"/>
-      <c r="O19" s="143"/>
-      <c r="P19" s="143"/>
-      <c r="Q19" s="143"/>
-      <c r="R19" s="143"/>
-      <c r="S19" s="143"/>
+      <c r="N19" s="153"/>
+      <c r="O19" s="153"/>
+      <c r="P19" s="153"/>
+      <c r="Q19" s="153"/>
+      <c r="R19" s="153"/>
+      <c r="S19" s="153"/>
       <c r="T19" s="154"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="171"/>
-      <c r="B20" s="172"/>
-      <c r="C20" s="172"/>
-      <c r="D20" s="173"/>
-      <c r="E20" s="178"/>
-      <c r="F20" s="170"/>
-      <c r="G20" s="158"/>
-      <c r="H20" s="158"/>
-      <c r="I20" s="159"/>
-      <c r="J20" s="157"/>
-      <c r="K20" s="158"/>
-      <c r="L20" s="159"/>
-      <c r="M20" s="157"/>
-      <c r="N20" s="158"/>
-      <c r="O20" s="158"/>
-      <c r="P20" s="158"/>
-      <c r="Q20" s="158"/>
-      <c r="R20" s="158"/>
-      <c r="S20" s="158"/>
-      <c r="T20" s="163"/>
+      <c r="A20" s="143"/>
+      <c r="B20" s="144"/>
+      <c r="C20" s="144"/>
+      <c r="D20" s="145"/>
+      <c r="E20" s="189"/>
+      <c r="F20" s="184"/>
+      <c r="G20" s="175"/>
+      <c r="H20" s="175"/>
+      <c r="I20" s="176"/>
+      <c r="J20" s="174"/>
+      <c r="K20" s="175"/>
+      <c r="L20" s="176"/>
+      <c r="M20" s="174"/>
+      <c r="N20" s="175"/>
+      <c r="O20" s="175"/>
+      <c r="P20" s="175"/>
+      <c r="Q20" s="175"/>
+      <c r="R20" s="175"/>
+      <c r="S20" s="175"/>
+      <c r="T20" s="180"/>
       <c r="V20" s="87" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21" s="171"/>
-      <c r="B21" s="172"/>
-      <c r="C21" s="172"/>
-      <c r="D21" s="173"/>
-      <c r="E21" s="178"/>
-      <c r="F21" s="170"/>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="159"/>
-      <c r="J21" s="157"/>
-      <c r="K21" s="158"/>
-      <c r="L21" s="159"/>
-      <c r="M21" s="157"/>
-      <c r="N21" s="158"/>
-      <c r="O21" s="158"/>
-      <c r="P21" s="158"/>
-      <c r="Q21" s="158"/>
-      <c r="R21" s="158"/>
-      <c r="S21" s="158"/>
-      <c r="T21" s="163"/>
+      <c r="A21" s="143"/>
+      <c r="B21" s="144"/>
+      <c r="C21" s="144"/>
+      <c r="D21" s="145"/>
+      <c r="E21" s="189"/>
+      <c r="F21" s="184"/>
+      <c r="G21" s="175"/>
+      <c r="H21" s="175"/>
+      <c r="I21" s="176"/>
+      <c r="J21" s="174"/>
+      <c r="K21" s="175"/>
+      <c r="L21" s="176"/>
+      <c r="M21" s="174"/>
+      <c r="N21" s="175"/>
+      <c r="O21" s="175"/>
+      <c r="P21" s="175"/>
+      <c r="Q21" s="175"/>
+      <c r="R21" s="175"/>
+      <c r="S21" s="175"/>
+      <c r="T21" s="180"/>
       <c r="V21" s="87" t="s">
         <v>58</v>
       </c>
@@ -5706,26 +5712,26 @@
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" s="171"/>
-      <c r="B22" s="172"/>
-      <c r="C22" s="172"/>
-      <c r="D22" s="173"/>
-      <c r="E22" s="178"/>
-      <c r="F22" s="170"/>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="159"/>
-      <c r="J22" s="157"/>
-      <c r="K22" s="158"/>
-      <c r="L22" s="159"/>
-      <c r="M22" s="157"/>
-      <c r="N22" s="158"/>
-      <c r="O22" s="158"/>
-      <c r="P22" s="158"/>
-      <c r="Q22" s="158"/>
-      <c r="R22" s="158"/>
-      <c r="S22" s="158"/>
-      <c r="T22" s="163"/>
+      <c r="A22" s="143"/>
+      <c r="B22" s="144"/>
+      <c r="C22" s="144"/>
+      <c r="D22" s="145"/>
+      <c r="E22" s="189"/>
+      <c r="F22" s="184"/>
+      <c r="G22" s="175"/>
+      <c r="H22" s="175"/>
+      <c r="I22" s="176"/>
+      <c r="J22" s="174"/>
+      <c r="K22" s="175"/>
+      <c r="L22" s="176"/>
+      <c r="M22" s="174"/>
+      <c r="N22" s="175"/>
+      <c r="O22" s="175"/>
+      <c r="P22" s="175"/>
+      <c r="Q22" s="175"/>
+      <c r="R22" s="175"/>
+      <c r="S22" s="175"/>
+      <c r="T22" s="180"/>
       <c r="V22" s="88" t="s">
         <v>224</v>
       </c>
@@ -5737,26 +5743,26 @@
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A23" s="171"/>
-      <c r="B23" s="172"/>
-      <c r="C23" s="172"/>
-      <c r="D23" s="173"/>
-      <c r="E23" s="178"/>
-      <c r="F23" s="170"/>
-      <c r="G23" s="158"/>
-      <c r="H23" s="158"/>
-      <c r="I23" s="159"/>
-      <c r="J23" s="157"/>
-      <c r="K23" s="158"/>
-      <c r="L23" s="159"/>
-      <c r="M23" s="157"/>
-      <c r="N23" s="158"/>
-      <c r="O23" s="158"/>
-      <c r="P23" s="158"/>
-      <c r="Q23" s="158"/>
-      <c r="R23" s="158"/>
-      <c r="S23" s="158"/>
-      <c r="T23" s="163"/>
+      <c r="A23" s="143"/>
+      <c r="B23" s="144"/>
+      <c r="C23" s="144"/>
+      <c r="D23" s="145"/>
+      <c r="E23" s="189"/>
+      <c r="F23" s="184"/>
+      <c r="G23" s="175"/>
+      <c r="H23" s="175"/>
+      <c r="I23" s="176"/>
+      <c r="J23" s="174"/>
+      <c r="K23" s="175"/>
+      <c r="L23" s="176"/>
+      <c r="M23" s="174"/>
+      <c r="N23" s="175"/>
+      <c r="O23" s="175"/>
+      <c r="P23" s="175"/>
+      <c r="Q23" s="175"/>
+      <c r="R23" s="175"/>
+      <c r="S23" s="175"/>
+      <c r="T23" s="180"/>
       <c r="V23" s="88" t="s">
         <v>225</v>
       </c>
@@ -5765,26 +5771,26 @@
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A24" s="171"/>
-      <c r="B24" s="172"/>
-      <c r="C24" s="172"/>
-      <c r="D24" s="173"/>
-      <c r="E24" s="178"/>
-      <c r="F24" s="170"/>
-      <c r="G24" s="158"/>
-      <c r="H24" s="158"/>
-      <c r="I24" s="159"/>
-      <c r="J24" s="157"/>
-      <c r="K24" s="158"/>
-      <c r="L24" s="159"/>
-      <c r="M24" s="157"/>
-      <c r="N24" s="158"/>
-      <c r="O24" s="158"/>
-      <c r="P24" s="158"/>
-      <c r="Q24" s="158"/>
-      <c r="R24" s="158"/>
-      <c r="S24" s="158"/>
-      <c r="T24" s="163"/>
+      <c r="A24" s="143"/>
+      <c r="B24" s="144"/>
+      <c r="C24" s="144"/>
+      <c r="D24" s="145"/>
+      <c r="E24" s="189"/>
+      <c r="F24" s="184"/>
+      <c r="G24" s="175"/>
+      <c r="H24" s="175"/>
+      <c r="I24" s="176"/>
+      <c r="J24" s="174"/>
+      <c r="K24" s="175"/>
+      <c r="L24" s="176"/>
+      <c r="M24" s="174"/>
+      <c r="N24" s="175"/>
+      <c r="O24" s="175"/>
+      <c r="P24" s="175"/>
+      <c r="Q24" s="175"/>
+      <c r="R24" s="175"/>
+      <c r="S24" s="175"/>
+      <c r="T24" s="180"/>
       <c r="V24" s="88" t="s">
         <v>226</v>
       </c>
@@ -5793,26 +5799,26 @@
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" s="171"/>
-      <c r="B25" s="172"/>
-      <c r="C25" s="172"/>
-      <c r="D25" s="173"/>
-      <c r="E25" s="178"/>
-      <c r="F25" s="170"/>
-      <c r="G25" s="158"/>
-      <c r="H25" s="158"/>
-      <c r="I25" s="159"/>
-      <c r="J25" s="157"/>
-      <c r="K25" s="158"/>
-      <c r="L25" s="159"/>
-      <c r="M25" s="157"/>
-      <c r="N25" s="158"/>
-      <c r="O25" s="158"/>
-      <c r="P25" s="158"/>
-      <c r="Q25" s="158"/>
-      <c r="R25" s="158"/>
-      <c r="S25" s="158"/>
-      <c r="T25" s="163"/>
+      <c r="A25" s="143"/>
+      <c r="B25" s="144"/>
+      <c r="C25" s="144"/>
+      <c r="D25" s="145"/>
+      <c r="E25" s="189"/>
+      <c r="F25" s="184"/>
+      <c r="G25" s="175"/>
+      <c r="H25" s="175"/>
+      <c r="I25" s="176"/>
+      <c r="J25" s="174"/>
+      <c r="K25" s="175"/>
+      <c r="L25" s="176"/>
+      <c r="M25" s="174"/>
+      <c r="N25" s="175"/>
+      <c r="O25" s="175"/>
+      <c r="P25" s="175"/>
+      <c r="Q25" s="175"/>
+      <c r="R25" s="175"/>
+      <c r="S25" s="175"/>
+      <c r="T25" s="180"/>
       <c r="V25" s="88" t="s">
         <v>227</v>
       </c>
@@ -5821,231 +5827,221 @@
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" s="171"/>
-      <c r="B26" s="172"/>
-      <c r="C26" s="172"/>
-      <c r="D26" s="173"/>
-      <c r="E26" s="178"/>
-      <c r="F26" s="170"/>
-      <c r="G26" s="158"/>
-      <c r="H26" s="158"/>
-      <c r="I26" s="159"/>
-      <c r="J26" s="157"/>
-      <c r="K26" s="158"/>
-      <c r="L26" s="159"/>
-      <c r="M26" s="157"/>
-      <c r="N26" s="158"/>
-      <c r="O26" s="158"/>
-      <c r="P26" s="158"/>
-      <c r="Q26" s="158"/>
-      <c r="R26" s="158"/>
-      <c r="S26" s="158"/>
-      <c r="T26" s="163"/>
+      <c r="A26" s="143"/>
+      <c r="B26" s="144"/>
+      <c r="C26" s="144"/>
+      <c r="D26" s="145"/>
+      <c r="E26" s="189"/>
+      <c r="F26" s="184"/>
+      <c r="G26" s="175"/>
+      <c r="H26" s="175"/>
+      <c r="I26" s="176"/>
+      <c r="J26" s="174"/>
+      <c r="K26" s="175"/>
+      <c r="L26" s="176"/>
+      <c r="M26" s="174"/>
+      <c r="N26" s="175"/>
+      <c r="O26" s="175"/>
+      <c r="P26" s="175"/>
+      <c r="Q26" s="175"/>
+      <c r="R26" s="175"/>
+      <c r="S26" s="175"/>
+      <c r="T26" s="180"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" s="171"/>
-      <c r="B27" s="172"/>
-      <c r="C27" s="172"/>
-      <c r="D27" s="173"/>
-      <c r="E27" s="178"/>
-      <c r="F27" s="170"/>
-      <c r="G27" s="158"/>
-      <c r="H27" s="158"/>
-      <c r="I27" s="159"/>
-      <c r="J27" s="157"/>
-      <c r="K27" s="158"/>
-      <c r="L27" s="159"/>
-      <c r="M27" s="157"/>
-      <c r="N27" s="158"/>
-      <c r="O27" s="158"/>
-      <c r="P27" s="158"/>
-      <c r="Q27" s="158"/>
-      <c r="R27" s="158"/>
-      <c r="S27" s="158"/>
-      <c r="T27" s="163"/>
+      <c r="A27" s="143"/>
+      <c r="B27" s="144"/>
+      <c r="C27" s="144"/>
+      <c r="D27" s="145"/>
+      <c r="E27" s="189"/>
+      <c r="F27" s="184"/>
+      <c r="G27" s="175"/>
+      <c r="H27" s="175"/>
+      <c r="I27" s="176"/>
+      <c r="J27" s="174"/>
+      <c r="K27" s="175"/>
+      <c r="L27" s="176"/>
+      <c r="M27" s="174"/>
+      <c r="N27" s="175"/>
+      <c r="O27" s="175"/>
+      <c r="P27" s="175"/>
+      <c r="Q27" s="175"/>
+      <c r="R27" s="175"/>
+      <c r="S27" s="175"/>
+      <c r="T27" s="180"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" s="171"/>
-      <c r="B28" s="172"/>
-      <c r="C28" s="172"/>
-      <c r="D28" s="173"/>
-      <c r="E28" s="178"/>
-      <c r="F28" s="170"/>
-      <c r="G28" s="158"/>
-      <c r="H28" s="158"/>
-      <c r="I28" s="159"/>
-      <c r="J28" s="157"/>
-      <c r="K28" s="158"/>
-      <c r="L28" s="159"/>
-      <c r="M28" s="157"/>
-      <c r="N28" s="158"/>
-      <c r="O28" s="158"/>
-      <c r="P28" s="158"/>
-      <c r="Q28" s="158"/>
-      <c r="R28" s="158"/>
-      <c r="S28" s="158"/>
-      <c r="T28" s="163"/>
+      <c r="A28" s="143"/>
+      <c r="B28" s="144"/>
+      <c r="C28" s="144"/>
+      <c r="D28" s="145"/>
+      <c r="E28" s="189"/>
+      <c r="F28" s="184"/>
+      <c r="G28" s="175"/>
+      <c r="H28" s="175"/>
+      <c r="I28" s="176"/>
+      <c r="J28" s="174"/>
+      <c r="K28" s="175"/>
+      <c r="L28" s="176"/>
+      <c r="M28" s="174"/>
+      <c r="N28" s="175"/>
+      <c r="O28" s="175"/>
+      <c r="P28" s="175"/>
+      <c r="Q28" s="175"/>
+      <c r="R28" s="175"/>
+      <c r="S28" s="175"/>
+      <c r="T28" s="180"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A29" s="171"/>
-      <c r="B29" s="172"/>
-      <c r="C29" s="172"/>
-      <c r="D29" s="173"/>
-      <c r="E29" s="178"/>
-      <c r="F29" s="170"/>
-      <c r="G29" s="158"/>
-      <c r="H29" s="158"/>
-      <c r="I29" s="159"/>
-      <c r="J29" s="157"/>
-      <c r="K29" s="158"/>
-      <c r="L29" s="159"/>
-      <c r="M29" s="157"/>
-      <c r="N29" s="158"/>
-      <c r="O29" s="158"/>
-      <c r="P29" s="158"/>
-      <c r="Q29" s="158"/>
-      <c r="R29" s="158"/>
-      <c r="S29" s="158"/>
-      <c r="T29" s="163"/>
+      <c r="A29" s="143"/>
+      <c r="B29" s="144"/>
+      <c r="C29" s="144"/>
+      <c r="D29" s="145"/>
+      <c r="E29" s="189"/>
+      <c r="F29" s="184"/>
+      <c r="G29" s="175"/>
+      <c r="H29" s="175"/>
+      <c r="I29" s="176"/>
+      <c r="J29" s="174"/>
+      <c r="K29" s="175"/>
+      <c r="L29" s="176"/>
+      <c r="M29" s="174"/>
+      <c r="N29" s="175"/>
+      <c r="O29" s="175"/>
+      <c r="P29" s="175"/>
+      <c r="Q29" s="175"/>
+      <c r="R29" s="175"/>
+      <c r="S29" s="175"/>
+      <c r="T29" s="180"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="171"/>
-      <c r="B30" s="172"/>
-      <c r="C30" s="172"/>
-      <c r="D30" s="173"/>
-      <c r="E30" s="178"/>
-      <c r="F30" s="170"/>
-      <c r="G30" s="158"/>
-      <c r="H30" s="158"/>
-      <c r="I30" s="159"/>
-      <c r="J30" s="157"/>
-      <c r="K30" s="158"/>
-      <c r="L30" s="159"/>
-      <c r="M30" s="157"/>
-      <c r="N30" s="158"/>
-      <c r="O30" s="158"/>
-      <c r="P30" s="158"/>
-      <c r="Q30" s="158"/>
-      <c r="R30" s="158"/>
-      <c r="S30" s="158"/>
-      <c r="T30" s="163"/>
+      <c r="A30" s="143"/>
+      <c r="B30" s="144"/>
+      <c r="C30" s="144"/>
+      <c r="D30" s="145"/>
+      <c r="E30" s="189"/>
+      <c r="F30" s="184"/>
+      <c r="G30" s="175"/>
+      <c r="H30" s="175"/>
+      <c r="I30" s="176"/>
+      <c r="J30" s="174"/>
+      <c r="K30" s="175"/>
+      <c r="L30" s="176"/>
+      <c r="M30" s="174"/>
+      <c r="N30" s="175"/>
+      <c r="O30" s="175"/>
+      <c r="P30" s="175"/>
+      <c r="Q30" s="175"/>
+      <c r="R30" s="175"/>
+      <c r="S30" s="175"/>
+      <c r="T30" s="180"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A31" s="171"/>
-      <c r="B31" s="172"/>
-      <c r="C31" s="172"/>
-      <c r="D31" s="173"/>
-      <c r="E31" s="178"/>
-      <c r="F31" s="170"/>
-      <c r="G31" s="158"/>
-      <c r="H31" s="158"/>
-      <c r="I31" s="159"/>
-      <c r="J31" s="157"/>
-      <c r="K31" s="158"/>
-      <c r="L31" s="159"/>
-      <c r="M31" s="157"/>
-      <c r="N31" s="158"/>
-      <c r="O31" s="158"/>
-      <c r="P31" s="158"/>
-      <c r="Q31" s="158"/>
-      <c r="R31" s="158"/>
-      <c r="S31" s="158"/>
-      <c r="T31" s="163"/>
+      <c r="A31" s="143"/>
+      <c r="B31" s="144"/>
+      <c r="C31" s="144"/>
+      <c r="D31" s="145"/>
+      <c r="E31" s="189"/>
+      <c r="F31" s="184"/>
+      <c r="G31" s="175"/>
+      <c r="H31" s="175"/>
+      <c r="I31" s="176"/>
+      <c r="J31" s="174"/>
+      <c r="K31" s="175"/>
+      <c r="L31" s="176"/>
+      <c r="M31" s="174"/>
+      <c r="N31" s="175"/>
+      <c r="O31" s="175"/>
+      <c r="P31" s="175"/>
+      <c r="Q31" s="175"/>
+      <c r="R31" s="175"/>
+      <c r="S31" s="175"/>
+      <c r="T31" s="180"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A32" s="171"/>
-      <c r="B32" s="172"/>
-      <c r="C32" s="172"/>
-      <c r="D32" s="173"/>
-      <c r="E32" s="178"/>
-      <c r="F32" s="170"/>
-      <c r="G32" s="158"/>
-      <c r="H32" s="158"/>
-      <c r="I32" s="159"/>
-      <c r="J32" s="157"/>
-      <c r="K32" s="158"/>
-      <c r="L32" s="159"/>
-      <c r="M32" s="157"/>
-      <c r="N32" s="158"/>
-      <c r="O32" s="158"/>
-      <c r="P32" s="158"/>
-      <c r="Q32" s="158"/>
-      <c r="R32" s="158"/>
-      <c r="S32" s="158"/>
-      <c r="T32" s="163"/>
+      <c r="A32" s="143"/>
+      <c r="B32" s="144"/>
+      <c r="C32" s="144"/>
+      <c r="D32" s="145"/>
+      <c r="E32" s="189"/>
+      <c r="F32" s="184"/>
+      <c r="G32" s="175"/>
+      <c r="H32" s="175"/>
+      <c r="I32" s="176"/>
+      <c r="J32" s="174"/>
+      <c r="K32" s="175"/>
+      <c r="L32" s="176"/>
+      <c r="M32" s="174"/>
+      <c r="N32" s="175"/>
+      <c r="O32" s="175"/>
+      <c r="P32" s="175"/>
+      <c r="Q32" s="175"/>
+      <c r="R32" s="175"/>
+      <c r="S32" s="175"/>
+      <c r="T32" s="180"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="171"/>
-      <c r="B33" s="172"/>
-      <c r="C33" s="172"/>
-      <c r="D33" s="173"/>
-      <c r="E33" s="178"/>
-      <c r="F33" s="170"/>
-      <c r="G33" s="158"/>
-      <c r="H33" s="158"/>
-      <c r="I33" s="159"/>
-      <c r="J33" s="157"/>
-      <c r="K33" s="158"/>
-      <c r="L33" s="159"/>
-      <c r="M33" s="157"/>
-      <c r="N33" s="158"/>
-      <c r="O33" s="158"/>
-      <c r="P33" s="158"/>
-      <c r="Q33" s="158"/>
-      <c r="R33" s="158"/>
-      <c r="S33" s="158"/>
-      <c r="T33" s="163"/>
+      <c r="A33" s="143"/>
+      <c r="B33" s="144"/>
+      <c r="C33" s="144"/>
+      <c r="D33" s="145"/>
+      <c r="E33" s="189"/>
+      <c r="F33" s="184"/>
+      <c r="G33" s="175"/>
+      <c r="H33" s="175"/>
+      <c r="I33" s="176"/>
+      <c r="J33" s="174"/>
+      <c r="K33" s="175"/>
+      <c r="L33" s="176"/>
+      <c r="M33" s="174"/>
+      <c r="N33" s="175"/>
+      <c r="O33" s="175"/>
+      <c r="P33" s="175"/>
+      <c r="Q33" s="175"/>
+      <c r="R33" s="175"/>
+      <c r="S33" s="175"/>
+      <c r="T33" s="180"/>
     </row>
     <row r="34" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="174"/>
-      <c r="B34" s="175"/>
-      <c r="C34" s="175"/>
-      <c r="D34" s="176"/>
-      <c r="E34" s="179"/>
-      <c r="F34" s="180"/>
-      <c r="G34" s="161"/>
-      <c r="H34" s="161"/>
-      <c r="I34" s="162"/>
-      <c r="J34" s="160"/>
-      <c r="K34" s="161"/>
-      <c r="L34" s="162"/>
-      <c r="M34" s="160"/>
-      <c r="N34" s="161"/>
-      <c r="O34" s="161"/>
-      <c r="P34" s="161"/>
-      <c r="Q34" s="161"/>
-      <c r="R34" s="161"/>
-      <c r="S34" s="161"/>
-      <c r="T34" s="164"/>
+      <c r="A34" s="185"/>
+      <c r="B34" s="186"/>
+      <c r="C34" s="186"/>
+      <c r="D34" s="187"/>
+      <c r="E34" s="190"/>
+      <c r="F34" s="191"/>
+      <c r="G34" s="178"/>
+      <c r="H34" s="178"/>
+      <c r="I34" s="179"/>
+      <c r="J34" s="177"/>
+      <c r="K34" s="178"/>
+      <c r="L34" s="179"/>
+      <c r="M34" s="177"/>
+      <c r="N34" s="178"/>
+      <c r="O34" s="178"/>
+      <c r="P34" s="178"/>
+      <c r="Q34" s="178"/>
+      <c r="R34" s="178"/>
+      <c r="S34" s="178"/>
+      <c r="T34" s="181"/>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="A13:D14"/>
-    <mergeCell ref="A15:D18"/>
-    <mergeCell ref="A7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="M7:T8"/>
-    <mergeCell ref="O6:T6"/>
-    <mergeCell ref="M5:P5"/>
-    <mergeCell ref="Q5:T5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="I7:L8"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="Q3:T3"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="I11:L12"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
     <mergeCell ref="M11:T12"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="A9:B9"/>
@@ -6062,22 +6058,32 @@
     <mergeCell ref="A19:D34"/>
     <mergeCell ref="E19:E34"/>
     <mergeCell ref="F19:I34"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="I11:L12"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="Q3:T3"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="M7:T8"/>
+    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="M5:P5"/>
+    <mergeCell ref="Q5:T5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="I7:L8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="A13:D14"/>
+    <mergeCell ref="A15:D18"/>
+    <mergeCell ref="A7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6617,7 +6623,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F17"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>